<commit_message>
Update project with surrogate Pareto optimization and README
</commit_message>
<xml_diff>
--- a/pareto_optimal_nsga2_krg.xlsx
+++ b/pareto_optimal_nsga2_krg.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ParetoOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0A93D2-8FCE-42E8-9280-230AA623F9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3B4536-05E5-4E3A-86C8-691E995D7332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13275" yWindow="2160" windowWidth="6735" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -399,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="M193" sqref="M193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,3402 +437,3402 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14.999999999689379</v>
+        <v>14.945118492183409</v>
       </c>
       <c r="B2">
-        <v>0.36914838304321701</v>
+        <v>0.36326267444459209</v>
       </c>
       <c r="C2">
-        <v>40.060056865434262</v>
+        <v>40.190298333485153</v>
       </c>
       <c r="D2">
-        <v>0.91508360741210326</v>
+        <v>0.91493036735587019</v>
       </c>
       <c r="E2">
-        <v>8.556442949137038</v>
+        <v>8.5257143928328638</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>14.999999999753371</v>
+        <v>14.945118505848731</v>
       </c>
       <c r="B3">
-        <v>0.89999999998472513</v>
+        <v>0.89755336772676075</v>
       </c>
       <c r="C3">
-        <v>59.999999824861703</v>
+        <v>59.948283826427051</v>
       </c>
       <c r="D3">
-        <v>0.56240320372435826</v>
+        <v>0.562607687196374</v>
       </c>
       <c r="E3">
-        <v>13.886239138918951</v>
+        <v>13.86982844597811</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14.997489255876911</v>
+        <v>14.94511844683395</v>
       </c>
       <c r="B4">
-        <v>0.56127164248866757</v>
+        <v>0.8403229172952803</v>
       </c>
       <c r="C4">
-        <v>40.119541889771988</v>
+        <v>43.711986247580263</v>
       </c>
       <c r="D4">
-        <v>0.90533552295888498</v>
+        <v>0.83702014629085608</v>
       </c>
       <c r="E4">
-        <v>9.4780992128597426</v>
+        <v>10.917006958972321</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14.999999999757449</v>
+        <v>14.94511816865915</v>
       </c>
       <c r="B5">
-        <v>0.87859783862669938</v>
+        <v>0.89712958251148789</v>
       </c>
       <c r="C5">
-        <v>57.937900954473157</v>
+        <v>58.711514814158598</v>
       </c>
       <c r="D5">
-        <v>0.62783642629696068</v>
+        <v>0.59654781917318034</v>
       </c>
       <c r="E5">
-        <v>13.531828192077491</v>
+        <v>13.71421532287448</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14.99999669987656</v>
+        <v>14.945118415578779</v>
       </c>
       <c r="B6">
-        <v>0.88937962442825802</v>
+        <v>0.89590231891387284</v>
       </c>
       <c r="C6">
-        <v>50.624601035667013</v>
+        <v>58.290129037563133</v>
       </c>
       <c r="D6">
-        <v>0.77304866928160954</v>
+        <v>0.60758210320038575</v>
       </c>
       <c r="E6">
-        <v>11.905278667704991</v>
+        <v>13.64782724598315</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>14.99999919977947</v>
+        <v>14.944687944872999</v>
       </c>
       <c r="B7">
-        <v>0.88860317983758119</v>
+        <v>0.84080854396593008</v>
       </c>
       <c r="C7">
-        <v>57.441662458459717</v>
+        <v>43.35247872525467</v>
       </c>
       <c r="D7">
-        <v>0.63233514515605549</v>
+        <v>0.84056784265416773</v>
       </c>
       <c r="E7">
-        <v>13.493823357310269</v>
+        <v>10.868384280882371</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14.99998799958105</v>
+        <v>14.945118301312959</v>
       </c>
       <c r="B8">
-        <v>0.89972251767929046</v>
+        <v>0.87987928763427348</v>
       </c>
       <c r="C8">
-        <v>59.091902309198858</v>
+        <v>57.337860392815053</v>
       </c>
       <c r="D8">
-        <v>0.58742011049210885</v>
+        <v>0.63758490809087009</v>
       </c>
       <c r="E8">
-        <v>13.78418727571219</v>
+        <v>13.41838472577532</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>14.99991381132743</v>
+        <v>14.94511792039636</v>
       </c>
       <c r="B9">
-        <v>0.53842978211430159</v>
+        <v>0.89712662076263583</v>
       </c>
       <c r="C9">
-        <v>40.008219335295472</v>
+        <v>48.954881653716278</v>
       </c>
       <c r="D9">
-        <v>0.90737552186638226</v>
+        <v>0.78823272391187771</v>
       </c>
       <c r="E9">
-        <v>9.3694449930867858</v>
+        <v>11.621776638923651</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>14.999998374716149</v>
+        <v>14.945118148037549</v>
       </c>
       <c r="B10">
-        <v>0.8994238304413078</v>
+        <v>0.85837286024387349</v>
       </c>
       <c r="C10">
-        <v>50.74698823796178</v>
+        <v>56.411548718713327</v>
       </c>
       <c r="D10">
-        <v>0.77019422183580777</v>
+        <v>0.66578746201166628</v>
       </c>
       <c r="E10">
-        <v>11.955668672650051</v>
+        <v>13.13993351634379</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>14.9999999739732</v>
+        <v>14.945118504532219</v>
       </c>
       <c r="B11">
-        <v>0.89995691236686803</v>
+        <v>0.74607297602380762</v>
       </c>
       <c r="C11">
-        <v>50.110316118692609</v>
+        <v>40.190298333485153</v>
       </c>
       <c r="D11">
-        <v>0.77834027670504013</v>
+        <v>0.88521782072092614</v>
       </c>
       <c r="E11">
-        <v>11.829384787259601</v>
+        <v>10.16154843152904</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14.999999764483951</v>
+        <v>14.945118425366511</v>
       </c>
       <c r="B12">
-        <v>0.87780029562729078</v>
+        <v>0.83007938119940561</v>
       </c>
       <c r="C12">
-        <v>44.363732214288937</v>
+        <v>41.789281697619693</v>
       </c>
       <c r="D12">
-        <v>0.82150098204421274</v>
+        <v>0.8599327939491852</v>
       </c>
       <c r="E12">
-        <v>11.15276517530139</v>
+        <v>10.602019438511361</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14.97321738497523</v>
+        <v>14.945113534363109</v>
       </c>
       <c r="B13">
-        <v>0.89673780617803855</v>
+        <v>0.71345166003283544</v>
       </c>
       <c r="C13">
-        <v>49.258222669350722</v>
+        <v>40.615834928545901</v>
       </c>
       <c r="D13">
-        <v>0.78639230860072573</v>
+        <v>0.88793819846717703</v>
       </c>
       <c r="E13">
-        <v>11.672320523722121</v>
+        <v>10.0877699846127</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14.99999999375664</v>
+        <v>14.94511850560122</v>
       </c>
       <c r="B14">
-        <v>0.8997556875092525</v>
+        <v>0.75556823801654616</v>
       </c>
       <c r="C14">
-        <v>59.28829385452697</v>
+        <v>40.304222791190668</v>
       </c>
       <c r="D14">
-        <v>0.58212638292919539</v>
+        <v>0.88354063600610888</v>
       </c>
       <c r="E14">
-        <v>13.8081236483763</v>
+        <v>10.198835546215591</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14.99999923757294</v>
+        <v>14.94511608492164</v>
       </c>
       <c r="B15">
-        <v>0.71997293786314642</v>
+        <v>0.87849457695579325</v>
       </c>
       <c r="C15">
-        <v>40.334839315276277</v>
+        <v>57.619888154700341</v>
       </c>
       <c r="D15">
-        <v>0.88878566029002359</v>
+        <v>0.63273576444003232</v>
       </c>
       <c r="E15">
-        <v>10.117160820535871</v>
+        <v>13.461519917982709</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14.999981385725601</v>
+        <v>14.945117499715471</v>
       </c>
       <c r="B16">
-        <v>0.81215745866170841</v>
+        <v>0.89704034851966474</v>
       </c>
       <c r="C16">
-        <v>56.66503995246606</v>
+        <v>52.423266639215342</v>
       </c>
       <c r="D16">
-        <v>0.68473715049371209</v>
+        <v>0.73714996748449368</v>
       </c>
       <c r="E16">
-        <v>12.98410309949641</v>
+        <v>12.338491266799791</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>14.999985530504389</v>
+        <v>14.94511849249812</v>
       </c>
       <c r="B17">
-        <v>0.45542486135485399</v>
+        <v>0.89755335601782138</v>
       </c>
       <c r="C17">
-        <v>40.035941927202323</v>
+        <v>59.705109830621907</v>
       </c>
       <c r="D17">
-        <v>0.91269222888438095</v>
+        <v>0.56942007200471911</v>
       </c>
       <c r="E17">
-        <v>8.9638868368661715</v>
+        <v>13.842702648300209</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>14.99997701683909</v>
+        <v>14.94504343615956</v>
       </c>
       <c r="B18">
-        <v>0.89702828614658792</v>
+        <v>0.89699691754721778</v>
       </c>
       <c r="C18">
-        <v>53.596354119287618</v>
+        <v>59.249539892057037</v>
       </c>
       <c r="D18">
-        <v>0.70836363875506425</v>
+        <v>0.58235424383488521</v>
       </c>
       <c r="E18">
-        <v>12.6726120977945</v>
+        <v>13.785653387709941</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14.999999997981581</v>
+        <v>14.94511835170089</v>
       </c>
       <c r="B19">
-        <v>0.77365290803758302</v>
+        <v>0.46088142224447709</v>
       </c>
       <c r="C19">
-        <v>40.417497864721128</v>
+        <v>40.19201469676608</v>
       </c>
       <c r="D19">
-        <v>0.88076648551623959</v>
+        <v>0.91184104267046129</v>
       </c>
       <c r="E19">
-        <v>10.292037739275839</v>
+        <v>8.9802058518162227</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14.99994945703806</v>
+        <v>14.9451055796986</v>
       </c>
       <c r="B20">
-        <v>0.61045183898550348</v>
+        <v>0.83080632461241066</v>
       </c>
       <c r="C20">
-        <v>40.513968038399788</v>
+        <v>57.277332226839427</v>
       </c>
       <c r="D20">
-        <v>0.89959127975532471</v>
+        <v>0.66453091554936361</v>
       </c>
       <c r="E20">
-        <v>9.7133365376263239</v>
+        <v>13.173171359997189</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>14.9999999758678</v>
+        <v>14.9451184568639</v>
       </c>
       <c r="B21">
-        <v>0.89710294835624382</v>
+        <v>0.893970218185409</v>
       </c>
       <c r="C21">
-        <v>53.098234130009899</v>
+        <v>58.550206524191402</v>
       </c>
       <c r="D21">
-        <v>0.72117984828704762</v>
+        <v>0.6023961111253</v>
       </c>
       <c r="E21">
-        <v>12.53891237973248</v>
+        <v>13.67838901217749</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>14.999999998457531</v>
+        <v>14.94511630392064</v>
       </c>
       <c r="B22">
-        <v>0.74656749995184823</v>
+        <v>0.89409045073814741</v>
       </c>
       <c r="C22">
-        <v>40.248784250833708</v>
+        <v>59.455615777341912</v>
       </c>
       <c r="D22">
-        <v>0.88542653793700621</v>
+        <v>0.57800678447762233</v>
       </c>
       <c r="E22">
-        <v>10.19611511446714</v>
+        <v>13.801660151616559</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>14.999999991017461</v>
+        <v>14.94510738197391</v>
       </c>
       <c r="B23">
-        <v>0.89652686591665554</v>
+        <v>0.88385067206477574</v>
       </c>
       <c r="C23">
-        <v>51.686954720090753</v>
+        <v>50.666542573395972</v>
       </c>
       <c r="D23">
-        <v>0.75420026090215619</v>
+        <v>0.77241816144635866</v>
       </c>
       <c r="E23">
-        <v>12.16703657188641</v>
+        <v>11.88093105958243</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>14.999998572024779</v>
+        <v>14.94511313572082</v>
       </c>
       <c r="B24">
-        <v>0.87878450486572324</v>
+        <v>0.77393252932812118</v>
       </c>
       <c r="C24">
-        <v>41.725427876658117</v>
+        <v>40.69934390277831</v>
       </c>
       <c r="D24">
-        <v>0.84953846542063394</v>
+        <v>0.87903071107282327</v>
       </c>
       <c r="E24">
-        <v>10.7736742565315</v>
+        <v>10.29008781383256</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>14.999999999197829</v>
+        <v>14.94511558107353</v>
       </c>
       <c r="B25">
-        <v>0.89628146307873924</v>
+        <v>0.81967610500543153</v>
       </c>
       <c r="C25">
-        <v>59.05988771319339</v>
+        <v>57.240430132506333</v>
       </c>
       <c r="D25">
-        <v>0.59006522185928867</v>
+        <v>0.67020548809931224</v>
       </c>
       <c r="E25">
-        <v>13.767806586886021</v>
+        <v>13.111982322323289</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14.99999999409278</v>
+        <v>14.94511848982156</v>
       </c>
       <c r="B26">
-        <v>0.80251580743944118</v>
+        <v>0.89418328985938533</v>
       </c>
       <c r="C26">
-        <v>40.742844159167127</v>
+        <v>50.732989370034169</v>
       </c>
       <c r="D26">
-        <v>0.87428093659741324</v>
+        <v>0.77032677405661709</v>
       </c>
       <c r="E26">
-        <v>10.41052177653329</v>
+        <v>11.92120597612846</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>14.99999999993455</v>
+        <v>14.94511849790616</v>
       </c>
       <c r="B27">
-        <v>0.89939177070075071</v>
+        <v>0.84933840947093919</v>
       </c>
       <c r="C27">
-        <v>52.983971382396241</v>
+        <v>57.702652824569839</v>
       </c>
       <c r="D27">
-        <v>0.72355839654286525</v>
+        <v>0.64680332676780494</v>
       </c>
       <c r="E27">
-        <v>12.51546981507482</v>
+        <v>13.341365111749839</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>14.99986244567938</v>
+        <v>14.94510956075028</v>
       </c>
       <c r="B28">
-        <v>0.8492790767212457</v>
+        <v>0.83301269216147433</v>
       </c>
       <c r="C28">
-        <v>46.437953590790123</v>
+        <v>41.403043382034532</v>
       </c>
       <c r="D28">
-        <v>0.81390572488255597</v>
+        <v>0.86304999726204934</v>
       </c>
       <c r="E28">
-        <v>11.2625190381455</v>
+        <v>10.556129116560941</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>14.99999997961344</v>
+        <v>14.945118239273519</v>
       </c>
       <c r="B29">
-        <v>0.81772831333077201</v>
+        <v>0.85848840205188615</v>
       </c>
       <c r="C29">
-        <v>42.141064398334713</v>
+        <v>57.356502188097487</v>
       </c>
       <c r="D29">
-        <v>0.85904179110095169</v>
+        <v>0.64920562099648982</v>
       </c>
       <c r="E29">
-        <v>10.642382950618529</v>
+        <v>13.32078738746741</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>14.97294470412745</v>
+        <v>14.94511170176404</v>
       </c>
       <c r="B30">
-        <v>0.88659746433302167</v>
+        <v>0.89577045075935569</v>
       </c>
       <c r="C30">
-        <v>49.008949683147307</v>
+        <v>51.331839694456221</v>
       </c>
       <c r="D30">
-        <v>0.78962484822747547</v>
+        <v>0.76039622158600917</v>
       </c>
       <c r="E30">
-        <v>11.61300210242827</v>
+        <v>12.059935508654039</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>14.999999999470059</v>
+        <v>14.945107269859291</v>
       </c>
       <c r="B31">
-        <v>0.89975284571934222</v>
+        <v>0.88296824341755398</v>
       </c>
       <c r="C31">
-        <v>52.884486457614791</v>
+        <v>52.413639155708388</v>
       </c>
       <c r="D31">
-        <v>0.72601223828117956</v>
+        <v>0.73998090240482683</v>
       </c>
       <c r="E31">
-        <v>12.48971281327654</v>
+        <v>12.292525388211271</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>14.999999737824581</v>
+        <v>14.94511835170089</v>
       </c>
       <c r="B32">
-        <v>0.88968568227665934</v>
+        <v>0.44835463070932219</v>
       </c>
       <c r="C32">
-        <v>43.761418309476149</v>
+        <v>40.19201469676608</v>
       </c>
       <c r="D32">
-        <v>0.82380546321380677</v>
+        <v>0.9125174112504274</v>
       </c>
       <c r="E32">
-        <v>11.11564563949597</v>
+        <v>8.9191800253554092</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>14.99997580653201</v>
+        <v>14.945088435232741</v>
       </c>
       <c r="B33">
-        <v>0.8996705678436242</v>
+        <v>0.40677188885976462</v>
       </c>
       <c r="C33">
-        <v>53.438865897657053</v>
+        <v>40.194640142687533</v>
       </c>
       <c r="D33">
-        <v>0.71169938568367641</v>
+        <v>0.91423578137163342</v>
       </c>
       <c r="E33">
-        <v>12.639479030547349</v>
+        <v>8.7206214801411335</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>14.999999662558089</v>
+        <v>14.945118160298779</v>
       </c>
       <c r="B34">
-        <v>0.84874019221030539</v>
+        <v>0.79478144316062416</v>
       </c>
       <c r="C34">
-        <v>57.6160027060766</v>
+        <v>56.411548718713327</v>
       </c>
       <c r="D34">
-        <v>0.65087473057772893</v>
+        <v>0.69357442300370986</v>
       </c>
       <c r="E34">
-        <v>13.34164064316106</v>
+        <v>12.822039686261521</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>14.99997297546569</v>
+        <v>14.945115931402761</v>
       </c>
       <c r="B35">
-        <v>0.46759515844028382</v>
+        <v>0.50398970582850489</v>
       </c>
       <c r="C35">
-        <v>40.000343443830673</v>
+        <v>40.19959164975559</v>
       </c>
       <c r="D35">
-        <v>0.91208695635008663</v>
+        <v>0.90907626080321857</v>
       </c>
       <c r="E35">
-        <v>9.0232836824134672</v>
+        <v>9.1906112838650689</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>14.99996169087273</v>
+        <v>14.945115462933609</v>
       </c>
       <c r="B36">
-        <v>0.89999999942382281</v>
+        <v>0.89088883562416021</v>
       </c>
       <c r="C36">
-        <v>49.929680236435182</v>
+        <v>56.797848935889093</v>
       </c>
       <c r="D36">
-        <v>0.78028158714994267</v>
+        <v>0.64111777919003587</v>
       </c>
       <c r="E36">
-        <v>11.796753583104479</v>
+        <v>13.37119182931224</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>14.9999845711456</v>
+        <v>14.94511612668531</v>
       </c>
       <c r="B37">
-        <v>0.83352806922889977</v>
+        <v>0.89747052946678096</v>
       </c>
       <c r="C37">
-        <v>46.157860655402892</v>
+        <v>53.06353418041892</v>
       </c>
       <c r="D37">
-        <v>0.81935939413953629</v>
+        <v>0.72110376688148592</v>
       </c>
       <c r="E37">
-        <v>11.187069275406961</v>
+        <v>12.51099988372118</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>14.99999999946586</v>
+        <v>14.94511313572082</v>
       </c>
       <c r="B38">
-        <v>0.89940041960562389</v>
+        <v>0.78798125041856082</v>
       </c>
       <c r="C38">
-        <v>52.80079270509583</v>
+        <v>40.69934390277831</v>
       </c>
       <c r="D38">
-        <v>0.72820588038703771</v>
+        <v>0.87671607686346509</v>
       </c>
       <c r="E38">
-        <v>12.466015525927091</v>
+        <v>10.332657593940031</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>14.999999999979311</v>
+        <v>14.944700471901291</v>
       </c>
       <c r="B39">
-        <v>0.84002685417354406</v>
+        <v>0.85363708607003563</v>
       </c>
       <c r="C39">
-        <v>45.033432551764633</v>
+        <v>57.726875897796504</v>
       </c>
       <c r="D39">
-        <v>0.82597575727543882</v>
+        <v>0.64406491331448368</v>
       </c>
       <c r="E39">
-        <v>11.10137604792339</v>
+        <v>13.3655583133311</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>14.999999999466951</v>
+        <v>14.94511845428722</v>
       </c>
       <c r="B40">
-        <v>0.89112093672765325</v>
+        <v>0.62949163338770542</v>
       </c>
       <c r="C40">
-        <v>51.600617879366808</v>
+        <v>40.191931934541913</v>
       </c>
       <c r="D40">
-        <v>0.75665228965005549</v>
+        <v>0.89872588294515598</v>
       </c>
       <c r="E40">
-        <v>12.13120096698446</v>
+        <v>9.753174146540923</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>14.99998370415247</v>
+        <v>14.94073851755727</v>
       </c>
       <c r="B41">
-        <v>0.86942797939407734</v>
+        <v>0.79562304724329147</v>
       </c>
       <c r="C41">
-        <v>48.774703721400513</v>
+        <v>56.575423902498507</v>
       </c>
       <c r="D41">
-        <v>0.79402422165540498</v>
+        <v>0.69081134125924715</v>
       </c>
       <c r="E41">
-        <v>11.54809304089264</v>
+        <v>12.85741442006379</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>14.999999999979311</v>
+        <v>14.94509882085911</v>
       </c>
       <c r="B42">
-        <v>0.81875531617456054</v>
+        <v>0.88687322025563975</v>
       </c>
       <c r="C42">
-        <v>45.033432551764633</v>
+        <v>59.074251680576523</v>
       </c>
       <c r="D42">
-        <v>0.83093860085249083</v>
+        <v>0.5922625525413544</v>
       </c>
       <c r="E42">
-        <v>11.02769341983597</v>
+        <v>13.72564018891039</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>14.999999955337559</v>
+        <v>14.945075742003411</v>
       </c>
       <c r="B43">
-        <v>0.84645015570687832</v>
+        <v>0.897550016203707</v>
       </c>
       <c r="C43">
-        <v>57.049764056143466</v>
+        <v>52.950579842898087</v>
       </c>
       <c r="D43">
-        <v>0.6629413341202175</v>
+        <v>0.72398106967174902</v>
       </c>
       <c r="E43">
-        <v>13.22614216297106</v>
+        <v>12.480843212922601</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>14.999980121912159</v>
+        <v>14.945118498818861</v>
       </c>
       <c r="B44">
-        <v>0.84729884432611069</v>
+        <v>0.8868159716890277</v>
       </c>
       <c r="C44">
-        <v>57.487937960966377</v>
+        <v>46.481352430539317</v>
       </c>
       <c r="D44">
-        <v>0.65424959120279813</v>
+        <v>0.80420034979500021</v>
       </c>
       <c r="E44">
-        <v>13.311569302620679</v>
+        <v>11.35847512090125</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>14.999999999757449</v>
+        <v>14.94501097728333</v>
       </c>
       <c r="B45">
-        <v>0.87843352980372447</v>
+        <v>0.77588891351168021</v>
       </c>
       <c r="C45">
-        <v>57.612438241294107</v>
+        <v>40.269464721952943</v>
       </c>
       <c r="D45">
-        <v>0.63490928364479726</v>
+        <v>0.88046555228335655</v>
       </c>
       <c r="E45">
-        <v>13.47676017041786</v>
+        <v>10.25627903463368</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>14.998150938021791</v>
+        <v>14.94511310100806</v>
       </c>
       <c r="B46">
-        <v>0.38763457889224201</v>
+        <v>0.8832976554849572</v>
       </c>
       <c r="C46">
-        <v>40.010329318282778</v>
+        <v>47.892821384960321</v>
       </c>
       <c r="D46">
-        <v>0.91495854216038242</v>
+        <v>0.79713275050620092</v>
       </c>
       <c r="E46">
-        <v>8.6372882320621578</v>
+        <v>11.467765890003511</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>14.99963657417932</v>
+        <v>14.94504189794214</v>
       </c>
       <c r="B47">
-        <v>0.63448352216976944</v>
+        <v>0.83487270565564997</v>
       </c>
       <c r="C47">
-        <v>40.078864032848038</v>
+        <v>57.337395936724803</v>
       </c>
       <c r="D47">
-        <v>0.89897536683409673</v>
+        <v>0.66146630714081911</v>
       </c>
       <c r="E47">
-        <v>9.7931752101833975</v>
+        <v>13.204311145599339</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>14.999999999788839</v>
+        <v>14.94511613557653</v>
       </c>
       <c r="B48">
-        <v>0.89986839581330302</v>
+        <v>0.62005424329322401</v>
       </c>
       <c r="C48">
-        <v>59.763610901753133</v>
+        <v>40.191778011276533</v>
       </c>
       <c r="D48">
-        <v>0.56898898380236507</v>
+        <v>0.89961498726185984</v>
       </c>
       <c r="E48">
-        <v>13.861780266429291</v>
+        <v>9.7149963131068979</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>14.99999991133328</v>
+        <v>14.94511834913321</v>
       </c>
       <c r="B49">
-        <v>0.78762552565553101</v>
+        <v>0.84177589960220278</v>
       </c>
       <c r="C49">
-        <v>40.33538211585094</v>
+        <v>44.640600214889247</v>
       </c>
       <c r="D49">
-        <v>0.87871190087626794</v>
+        <v>0.82829687815158837</v>
       </c>
       <c r="E49">
-        <v>10.32562833015637</v>
+        <v>11.03895933880225</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>14.999999768863979</v>
+        <v>14.94511838549241</v>
       </c>
       <c r="B50">
-        <v>0.80083526876980371</v>
+        <v>0.79837142983400766</v>
       </c>
       <c r="C50">
-        <v>57.052275940250617</v>
+        <v>56.845625898204013</v>
       </c>
       <c r="D50">
-        <v>0.68289801803915018</v>
+        <v>0.68574260198485659</v>
       </c>
       <c r="E50">
-        <v>13.00490518255396</v>
+        <v>12.92772882273615</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>14.999999990535301</v>
+        <v>14.945117784736629</v>
       </c>
       <c r="B51">
-        <v>0.8509487224557839</v>
+        <v>0.89109041633905739</v>
       </c>
       <c r="C51">
-        <v>43.201545712971487</v>
+        <v>47.296272079354253</v>
       </c>
       <c r="D51">
-        <v>0.8400350356961791</v>
+        <v>0.7988677033506898</v>
       </c>
       <c r="E51">
-        <v>10.90899782760601</v>
+        <v>11.435603773842271</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>14.9999997590473</v>
+        <v>14.945118415578779</v>
       </c>
       <c r="B52">
-        <v>0.80266408777034481</v>
+        <v>0.8139976035124411</v>
       </c>
       <c r="C52">
-        <v>56.559935644482067</v>
+        <v>56.575423902498507</v>
       </c>
       <c r="D52">
-        <v>0.69000775707741013</v>
+        <v>0.68379799128406116</v>
       </c>
       <c r="E52">
-        <v>12.915770846155899</v>
+        <v>12.95223041926093</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>14.999951051812371</v>
+        <v>14.945115923062049</v>
       </c>
       <c r="B53">
-        <v>0.89710150977415848</v>
+        <v>0.8630313807917086</v>
       </c>
       <c r="C53">
-        <v>59.404895163482742</v>
+        <v>42.432435968624667</v>
       </c>
       <c r="D53">
-        <v>0.58021135318824113</v>
+        <v>0.84543709988550031</v>
       </c>
       <c r="E53">
-        <v>13.813031371094141</v>
+        <v>10.805420944550139</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>14.99999674012655</v>
+        <v>14.94511816918704</v>
       </c>
       <c r="B54">
-        <v>0.84851695008325756</v>
+        <v>0.89737825772437729</v>
       </c>
       <c r="C54">
-        <v>41.814417653645037</v>
+        <v>58.550206524191402</v>
       </c>
       <c r="D54">
-        <v>0.85595575318967709</v>
+        <v>0.60044859015576324</v>
       </c>
       <c r="E54">
-        <v>10.69348871064544</v>
+        <v>13.69231330660571</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>14.99999981575125</v>
+        <v>14.94510738197391</v>
       </c>
       <c r="B55">
-        <v>0.8235281849124273</v>
+        <v>0.8941889018182243</v>
       </c>
       <c r="C55">
-        <v>41.450315858672909</v>
+        <v>49.349901295321558</v>
       </c>
       <c r="D55">
-        <v>0.86488480785068689</v>
+        <v>0.78563599129951933</v>
       </c>
       <c r="E55">
-        <v>10.56310624218737</v>
+        <v>11.67022069506937</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>14.99999946369484</v>
+        <v>14.945115872880271</v>
       </c>
       <c r="B56">
-        <v>0.88746406676450063</v>
+        <v>0.87872386524950374</v>
       </c>
       <c r="C56">
-        <v>59.113466455523508</v>
+        <v>43.093522657351222</v>
       </c>
       <c r="D56">
-        <v>0.59304182271207295</v>
+        <v>0.83381320984752982</v>
       </c>
       <c r="E56">
-        <v>13.74316081273483</v>
+        <v>10.95810293359113</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>14.999999987561679</v>
+        <v>14.94511792864049</v>
       </c>
       <c r="B57">
-        <v>0.83759040424298825</v>
+        <v>0.89579692661400812</v>
       </c>
       <c r="C57">
-        <v>56.646531704821939</v>
+        <v>53.427212924220591</v>
       </c>
       <c r="D57">
-        <v>0.67391325048345696</v>
+        <v>0.71212251064767507</v>
       </c>
       <c r="E57">
-        <v>13.106035641911481</v>
+        <v>12.60300436932393</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>14.99999701656643</v>
+        <v>14.94510697907727</v>
       </c>
       <c r="B58">
-        <v>0.82641799320639575</v>
+        <v>0.88405623317789439</v>
       </c>
       <c r="C58">
-        <v>57.259496301383962</v>
+        <v>52.954988454544271</v>
       </c>
       <c r="D58">
-        <v>0.66861053260701597</v>
+        <v>0.72695497685032773</v>
       </c>
       <c r="E58">
-        <v>13.16987485943171</v>
+        <v>12.4370943962384</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>14.999999972005829</v>
+        <v>14.94511790506583</v>
       </c>
       <c r="B59">
-        <v>0.50040722943793703</v>
+        <v>0.83236403787336699</v>
       </c>
       <c r="C59">
-        <v>40.018812756604937</v>
+        <v>41.893381773732642</v>
       </c>
       <c r="D59">
-        <v>0.91006519853412415</v>
+        <v>0.85837750438344285</v>
       </c>
       <c r="E59">
-        <v>9.1857756463063147</v>
+        <v>10.62452611629991</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>14.999999995812651</v>
+        <v>14.945118368603611</v>
       </c>
       <c r="B60">
-        <v>0.8972111461255089</v>
+        <v>0.86113400844067256</v>
       </c>
       <c r="C60">
-        <v>51.780525185501631</v>
+        <v>46.286000555471027</v>
       </c>
       <c r="D60">
-        <v>0.75219631342191395</v>
+        <v>0.81167905203788093</v>
       </c>
       <c r="E60">
-        <v>12.19224872082796</v>
+        <v>11.264642376419321</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>14.99999999941296</v>
+        <v>14.945118466213129</v>
       </c>
       <c r="B61">
-        <v>0.81576043779023333</v>
+        <v>0.89734836257353279</v>
       </c>
       <c r="C61">
-        <v>57.114627436671157</v>
+        <v>51.438775282047537</v>
       </c>
       <c r="D61">
-        <v>0.67587328863388585</v>
+        <v>0.75822371615113426</v>
       </c>
       <c r="E61">
-        <v>13.09028300886165</v>
+        <v>12.089570760921569</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>14.999999979273129</v>
+        <v>14.94511689810769</v>
       </c>
       <c r="B62">
-        <v>0.89640825501947052</v>
+        <v>0.85882517259263669</v>
       </c>
       <c r="C62">
-        <v>52.461333599862762</v>
+        <v>57.82761663911991</v>
       </c>
       <c r="D62">
-        <v>0.73713303023864285</v>
+        <v>0.63913275065391839</v>
       </c>
       <c r="E62">
-        <v>12.366128284205461</v>
+        <v>13.407668616072749</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>14.99999941743814</v>
+        <v>14.94511750578758</v>
       </c>
       <c r="B63">
-        <v>0.75404500321857582</v>
+        <v>0.82195627505404245</v>
       </c>
       <c r="C63">
-        <v>40.537785949282629</v>
+        <v>57.799678137253501</v>
       </c>
       <c r="D63">
-        <v>0.88328939470748802</v>
+        <v>0.65731204383768238</v>
       </c>
       <c r="E63">
-        <v>10.242708147372181</v>
+        <v>13.23287368252317</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>14.999999999769731</v>
+        <v>14.940729105843181</v>
       </c>
       <c r="B64">
-        <v>0.83015060226618564</v>
+        <v>0.67702877719828836</v>
       </c>
       <c r="C64">
-        <v>56.621218549166272</v>
+        <v>40.306687691260521</v>
       </c>
       <c r="D64">
-        <v>0.67771952211327824</v>
+        <v>0.89348257890157456</v>
       </c>
       <c r="E64">
-        <v>13.06459740494949</v>
+        <v>9.9373331964808447</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>14.99999954188063</v>
+        <v>14.945063621084509</v>
       </c>
       <c r="B65">
-        <v>0.88789979361116145</v>
+        <v>0.57819787626177965</v>
       </c>
       <c r="C65">
-        <v>58.917480194075793</v>
+        <v>40.2443469198004</v>
       </c>
       <c r="D65">
-        <v>0.59825685122221484</v>
+        <v>0.90315508541396405</v>
       </c>
       <c r="E65">
-        <v>13.718105893015609</v>
+        <v>9.5383416438780682</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>14.9999978484278</v>
+        <v>14.94511827206354</v>
       </c>
       <c r="B66">
-        <v>0.88756115356225918</v>
+        <v>0.89750190018999465</v>
       </c>
       <c r="C66">
-        <v>42.987766606747307</v>
+        <v>52.493325357648757</v>
       </c>
       <c r="D66">
-        <v>0.83285228662012734</v>
+        <v>0.73538077899748044</v>
       </c>
       <c r="E66">
-        <v>10.9982712428928</v>
+        <v>12.358423163169199</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>14.99999999969946</v>
+        <v>14.94511797686911</v>
       </c>
       <c r="B67">
-        <v>0.89167127132424673</v>
+        <v>0.86891329784772753</v>
       </c>
       <c r="C67">
-        <v>52.641713238144142</v>
+        <v>45.686173195684241</v>
       </c>
       <c r="D67">
-        <v>0.73373720339251891</v>
+        <v>0.81362709086584517</v>
       </c>
       <c r="E67">
-        <v>12.399419721094601</v>
+        <v>11.236695646694431</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>14.99999996095694</v>
+        <v>14.944257007770251</v>
       </c>
       <c r="B68">
-        <v>0.87878450486572324</v>
+        <v>0.88676856262853232</v>
       </c>
       <c r="C68">
-        <v>57.010736233758813</v>
+        <v>53.825351817798563</v>
       </c>
       <c r="D68">
-        <v>0.64623081745308175</v>
+        <v>0.70465081833451959</v>
       </c>
       <c r="E68">
-        <v>13.37218595583497</v>
+        <v>12.674607256395079</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>14.999999996835349</v>
+        <v>14.94511849977545</v>
       </c>
       <c r="B69">
-        <v>0.83818600397439535</v>
+        <v>0.88078793866341609</v>
       </c>
       <c r="C69">
-        <v>57.39820374155866</v>
+        <v>57.83852819066653</v>
       </c>
       <c r="D69">
-        <v>0.66049960985137002</v>
+        <v>0.6267445511911881</v>
       </c>
       <c r="E69">
-        <v>13.25218710765847</v>
+        <v>13.509314987210139</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>14.9999997733205</v>
+        <v>14.94510968775843</v>
       </c>
       <c r="B70">
-        <v>0.88992425937957342</v>
+        <v>0.83561553240239339</v>
       </c>
       <c r="C70">
-        <v>53.972901661517859</v>
+        <v>42.008286207363341</v>
       </c>
       <c r="D70">
-        <v>0.7010676178432349</v>
+        <v>0.85646861795734486</v>
       </c>
       <c r="E70">
-        <v>12.74582168540417</v>
+        <v>10.65196565961365</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>14.999866055701959</v>
+        <v>14.945112976592871</v>
       </c>
       <c r="B71">
-        <v>0.89888605619221862</v>
+        <v>0.87642330234289445</v>
       </c>
       <c r="C71">
-        <v>58.271136307118411</v>
+        <v>44.804965771696807</v>
       </c>
       <c r="D71">
-        <v>0.60837645191597745</v>
+        <v>0.81788958302728554</v>
       </c>
       <c r="E71">
-        <v>13.670265547980399</v>
+        <v>11.17361877558721</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>14.999999853554771</v>
+        <v>14.945116156613841</v>
       </c>
       <c r="B72">
-        <v>0.89718790662773684</v>
+        <v>0.88622235845394637</v>
       </c>
       <c r="C72">
-        <v>59.532989467832458</v>
+        <v>57.842880686382088</v>
       </c>
       <c r="D72">
-        <v>0.57660159000667555</v>
+        <v>0.62346447595365651</v>
       </c>
       <c r="E72">
-        <v>13.82821990258992</v>
+        <v>13.53452879795101</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>14.99999999797565</v>
+        <v>14.944802774443181</v>
       </c>
       <c r="B73">
-        <v>0.78343392307876036</v>
+        <v>0.82881788923789346</v>
       </c>
       <c r="C73">
-        <v>56.326676483897863</v>
+        <v>56.430874362214666</v>
       </c>
       <c r="D73">
-        <v>0.69999207274397857</v>
+        <v>0.67960381833055838</v>
       </c>
       <c r="E73">
-        <v>12.77141122473043</v>
+        <v>12.99768863206641</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>14.99999999861452</v>
+        <v>14.94511834802497</v>
       </c>
       <c r="B74">
-        <v>0.89736175061480972</v>
+        <v>0.79379700069967229</v>
       </c>
       <c r="C74">
-        <v>52.35100089607414</v>
+        <v>56.216834289371228</v>
       </c>
       <c r="D74">
-        <v>0.73956341188918984</v>
+        <v>0.69656786296861595</v>
       </c>
       <c r="E74">
-        <v>12.33979991534081</v>
+        <v>12.77782308026339</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>14.999999885230819</v>
+        <v>14.945115426433841</v>
       </c>
       <c r="B75">
-        <v>0.84163696973709634</v>
+        <v>0.60892071706153073</v>
       </c>
       <c r="C75">
-        <v>44.688819186356397</v>
+        <v>40.241532358522598</v>
       </c>
       <c r="D75">
-        <v>0.82827280154393124</v>
+        <v>0.90047634506004914</v>
       </c>
       <c r="E75">
-        <v>11.06937794503777</v>
+        <v>9.6708387799576876</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>14.99999999975341</v>
+        <v>14.945115838669221</v>
       </c>
       <c r="B76">
-        <v>0.80599898025197558</v>
+        <v>0.38813907354092092</v>
       </c>
       <c r="C76">
-        <v>56.621218549166272</v>
+        <v>40.261948133923831</v>
       </c>
       <c r="D76">
-        <v>0.68783329075891542</v>
+        <v>0.91458450612814413</v>
       </c>
       <c r="E76">
-        <v>12.94468719021666</v>
+        <v>8.6379935489597806</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>14.99999622767611</v>
+        <v>14.94510669146031</v>
       </c>
       <c r="B77">
-        <v>0.86310078146367786</v>
+        <v>0.89753633928560017</v>
       </c>
       <c r="C77">
-        <v>56.372341940452273</v>
+        <v>59.831512722490316</v>
       </c>
       <c r="D77">
-        <v>0.6656495387970619</v>
+        <v>0.56588163569282945</v>
       </c>
       <c r="E77">
-        <v>13.17607015792578</v>
+        <v>13.856957217557669</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>14.999999978504491</v>
+        <v>14.945112976459599</v>
       </c>
       <c r="B78">
-        <v>0.83473708635607435</v>
+        <v>0.89572816102349939</v>
       </c>
       <c r="C78">
-        <v>56.852851058741649</v>
+        <v>47.800193594073853</v>
       </c>
       <c r="D78">
-        <v>0.67194419153029106</v>
+        <v>0.79529448762200727</v>
       </c>
       <c r="E78">
-        <v>13.131995776824461</v>
+        <v>11.49153900170753</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>14.9999999299507</v>
+        <v>14.94510697907727</v>
       </c>
       <c r="B79">
-        <v>0.81284086458564297</v>
+        <v>0.89735178711265562</v>
       </c>
       <c r="C79">
-        <v>56.890687172915797</v>
+        <v>52.135693674676872</v>
       </c>
       <c r="D79">
-        <v>0.680910788043811</v>
+        <v>0.74377557538414052</v>
       </c>
       <c r="E79">
-        <v>13.031991922783</v>
+        <v>12.264152590446111</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>14.99964211018332</v>
+        <v>14.94511614109706</v>
       </c>
       <c r="B80">
-        <v>0.58658294042138848</v>
+        <v>0.82001908729026807</v>
       </c>
       <c r="C80">
-        <v>40.000006536365149</v>
+        <v>56.802331028084438</v>
       </c>
       <c r="D80">
-        <v>0.90349334689395044</v>
+        <v>0.67772671871272072</v>
       </c>
       <c r="E80">
-        <v>9.5898247750201246</v>
+        <v>13.027345426852291</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>14.99999949480228</v>
+        <v>14.945118487430189</v>
       </c>
       <c r="B81">
-        <v>0.70011403061002642</v>
+        <v>0.88253689326297646</v>
       </c>
       <c r="C81">
-        <v>40.479756499889533</v>
+        <v>51.029393958496428</v>
       </c>
       <c r="D81">
-        <v>0.89064247334721891</v>
+        <v>0.76713340570228361</v>
       </c>
       <c r="E81">
-        <v>10.05955180749962</v>
+        <v>11.955538879768749</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>14.99999795091097</v>
+        <v>14.945118148037549</v>
       </c>
       <c r="B82">
-        <v>0.83665579375067123</v>
+        <v>0.79099288514382893</v>
       </c>
       <c r="C82">
-        <v>42.352246598528673</v>
+        <v>56.411548718713327</v>
       </c>
       <c r="D82">
-        <v>0.85276860396634058</v>
+        <v>0.69491920547920694</v>
       </c>
       <c r="E82">
-        <v>10.735782941252401</v>
+        <v>12.80267283575067</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>14.999959992558351</v>
+        <v>14.945112994783351</v>
       </c>
       <c r="B83">
-        <v>0.69026602491605038</v>
+        <v>0.89508186380489974</v>
       </c>
       <c r="C83">
-        <v>40.160286095692413</v>
+        <v>53.209829009592347</v>
       </c>
       <c r="D83">
-        <v>0.89290588499472545</v>
+        <v>0.71792923380731277</v>
       </c>
       <c r="E83">
-        <v>10.00553165582393</v>
+        <v>12.542275376819269</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>14.99999792043322</v>
+        <v>14.94511831867597</v>
       </c>
       <c r="B84">
-        <v>0.83665728392204353</v>
+        <v>0.89755027431356893</v>
       </c>
       <c r="C84">
-        <v>57.204019117322893</v>
+        <v>47.966924046463831</v>
       </c>
       <c r="D84">
-        <v>0.66493382917081789</v>
+        <v>0.79407335471290164</v>
       </c>
       <c r="E84">
-        <v>13.20833018442133</v>
+        <v>11.511777996657811</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>14.999999982693209</v>
+        <v>14.945115519358509</v>
       </c>
       <c r="B85">
-        <v>0.89989331237342607</v>
+        <v>0.89563248197510092</v>
       </c>
       <c r="C85">
-        <v>59.655436127164108</v>
+        <v>52.91182030714922</v>
       </c>
       <c r="D85">
-        <v>0.57197537775622431</v>
+        <v>0.72540551030401546</v>
       </c>
       <c r="E85">
-        <v>13.85028367879444</v>
+        <v>12.46420646775265</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>14.99999489369867</v>
+        <v>14.945103952300061</v>
       </c>
       <c r="B86">
-        <v>0.65659521474761062</v>
+        <v>0.88559777035894427</v>
       </c>
       <c r="C86">
-        <v>40.435632229263383</v>
+        <v>57.663908038576423</v>
       </c>
       <c r="D86">
-        <v>0.89558650696223974</v>
+        <v>0.62764359337096365</v>
       </c>
       <c r="E86">
-        <v>9.8966678007571378</v>
+        <v>13.50166244968071</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>14.97207681022379</v>
+        <v>14.945114331745611</v>
       </c>
       <c r="B87">
-        <v>0.8492790767212457</v>
+        <v>0.6881426844548475</v>
       </c>
       <c r="C87">
-        <v>57.368586319532042</v>
+        <v>40.198507761411889</v>
       </c>
       <c r="D87">
-        <v>0.65468449867854839</v>
+        <v>0.89261264684330754</v>
       </c>
       <c r="E87">
-        <v>13.28887602812018</v>
+        <v>9.9730803534443293</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>14.99999965512942</v>
+        <v>14.945041434883411</v>
       </c>
       <c r="B88">
-        <v>0.82663009632426265</v>
+        <v>0.83421320472743687</v>
       </c>
       <c r="C88">
-        <v>40.412623384725997</v>
+        <v>46.481352430539317</v>
       </c>
       <c r="D88">
-        <v>0.87115142577489568</v>
+        <v>0.81640604032548125</v>
       </c>
       <c r="E88">
-        <v>10.44317228734964</v>
+        <v>11.19512969212515</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>14.999999955337559</v>
+        <v>14.94511826019013</v>
       </c>
       <c r="B89">
-        <v>0.84645015570687832</v>
+        <v>0.42039494726305471</v>
       </c>
       <c r="C89">
-        <v>56.615623734084743</v>
+        <v>40.190315736646063</v>
       </c>
       <c r="D89">
-        <v>0.67015744669670962</v>
+        <v>0.91377778770983353</v>
       </c>
       <c r="E89">
-        <v>13.143239923091251</v>
+        <v>8.7846024537413125</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>14.9999978484278</v>
+        <v>14.944367624787439</v>
       </c>
       <c r="B90">
-        <v>0.87887089368604077</v>
+        <v>0.89748940838422941</v>
       </c>
       <c r="C90">
-        <v>57.487937960966377</v>
+        <v>59.146497495737997</v>
       </c>
       <c r="D90">
-        <v>0.63717280375030549</v>
+        <v>0.58488646574181091</v>
       </c>
       <c r="E90">
-        <v>13.457409570861349</v>
+        <v>13.77408731551758</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>14.9999999717738</v>
+        <v>14.945116306177461</v>
       </c>
       <c r="B91">
-        <v>0.89628146307873924</v>
+        <v>0.86312598708299948</v>
       </c>
       <c r="C91">
-        <v>51.867354206571001</v>
+        <v>42.690504723122629</v>
       </c>
       <c r="D91">
-        <v>0.75052366546501004</v>
+        <v>0.84246692580049187</v>
       </c>
       <c r="E91">
-        <v>12.21160774091179</v>
+        <v>10.84550699964624</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>14.999999998121851</v>
+        <v>14.945118064461431</v>
       </c>
       <c r="B92">
-        <v>0.76873271653621533</v>
+        <v>0.89704932371946111</v>
       </c>
       <c r="C92">
-        <v>40.060056865434262</v>
+        <v>51.129242402074453</v>
       </c>
       <c r="D92">
-        <v>0.88239363339174293</v>
+        <v>0.76377793735157884</v>
       </c>
       <c r="E92">
-        <v>10.24866216838296</v>
+        <v>12.01606555102069</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>14.999998041775831</v>
+        <v>14.945078838751179</v>
       </c>
       <c r="B93">
-        <v>0.89109363928056395</v>
+        <v>0.64069805177487593</v>
       </c>
       <c r="C93">
-        <v>50.413851137743258</v>
+        <v>40.202770625374349</v>
       </c>
       <c r="D93">
-        <v>0.77566750385091743</v>
+        <v>0.89760963940235949</v>
       </c>
       <c r="E93">
-        <v>11.866687796924619</v>
+        <v>9.797914107694055</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>14.99999998775122</v>
+        <v>14.945118368603611</v>
       </c>
       <c r="B94">
-        <v>0.8057033940766215</v>
+        <v>0.86113400844067256</v>
       </c>
       <c r="C94">
-        <v>42.011959544102922</v>
+        <v>47.722284200893156</v>
       </c>
       <c r="D94">
-        <v>0.86274006182664098</v>
+        <v>0.80224907818517655</v>
       </c>
       <c r="E94">
-        <v>10.58416774038556</v>
+        <v>11.389961619749201</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>14.99999516968224</v>
+        <v>14.945108735747089</v>
       </c>
       <c r="B95">
-        <v>0.8915726495427494</v>
+        <v>0.83116433947469037</v>
       </c>
       <c r="C95">
-        <v>52.081107763888177</v>
+        <v>42.566724212507957</v>
       </c>
       <c r="D95">
-        <v>0.7466687662896887</v>
+        <v>0.85129652171990555</v>
       </c>
       <c r="E95">
-        <v>12.25280669970839</v>
+        <v>10.720652308550379</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>14.99999907810769</v>
+        <v>14.945118210154581</v>
       </c>
       <c r="B96">
-        <v>0.89995597405704975</v>
+        <v>0.82642409879981593</v>
       </c>
       <c r="C96">
-        <v>52.484636100468911</v>
+        <v>56.705763294954487</v>
       </c>
       <c r="D96">
-        <v>0.73589853031482599</v>
+        <v>0.67646264473598161</v>
       </c>
       <c r="E96">
-        <v>12.38286898101237</v>
+        <v>13.04019844100212</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>14.999979385999801</v>
+        <v>14.945117908375749</v>
       </c>
       <c r="B97">
-        <v>0.78371900325565635</v>
+        <v>0.89709859673916215</v>
       </c>
       <c r="C97">
-        <v>56.677671446781218</v>
+        <v>42.914908473128207</v>
       </c>
       <c r="D97">
-        <v>0.6949963838046026</v>
+        <v>0.83071738897805414</v>
       </c>
       <c r="E97">
-        <v>12.8437836905689</v>
+        <v>10.991060580450609</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>14.999999959490619</v>
+        <v>14.94511748347735</v>
       </c>
       <c r="B98">
-        <v>0.7943539530391972</v>
+        <v>0.89750190018999465</v>
       </c>
       <c r="C98">
-        <v>56.641126100297932</v>
+        <v>52.225849566428472</v>
       </c>
       <c r="D98">
-        <v>0.69188046932494907</v>
+        <v>0.74169421409524516</v>
       </c>
       <c r="E98">
-        <v>12.89016377919638</v>
+        <v>12.288035550835</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>14.999995620283441</v>
+        <v>14.94511786293128</v>
       </c>
       <c r="B99">
-        <v>0.8915726495427494</v>
+        <v>0.51812742709678816</v>
       </c>
       <c r="C99">
-        <v>58.279542105928158</v>
+        <v>40.205259872412348</v>
       </c>
       <c r="D99">
-        <v>0.612493006296571</v>
+        <v>0.90804621487581605</v>
       </c>
       <c r="E99">
-        <v>13.641053594878439</v>
+        <v>9.2588911330042105</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>14.999999739479851</v>
+        <v>14.94511650814991</v>
       </c>
       <c r="B100">
-        <v>0.85639656245538087</v>
+        <v>0.89734639647718295</v>
       </c>
       <c r="C100">
-        <v>43.6017682849875</v>
+        <v>51.843575851070248</v>
       </c>
       <c r="D100">
-        <v>0.83446594350666792</v>
+        <v>0.75015714331114258</v>
       </c>
       <c r="E100">
-        <v>10.98372027543126</v>
+        <v>12.18939501599807</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>14.999999586705369</v>
+        <v>14.940200190180709</v>
       </c>
       <c r="B101">
-        <v>0.89620961712280789</v>
+        <v>0.79896738812483559</v>
       </c>
       <c r="C101">
-        <v>49.544413449813618</v>
+        <v>56.575423902498507</v>
       </c>
       <c r="D101">
-        <v>0.7844045041643869</v>
+        <v>0.68956249510689138</v>
       </c>
       <c r="E101">
-        <v>11.72350020056224</v>
+        <v>12.874169372568909</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>14.99999988108886</v>
+        <v>14.945108312241169</v>
       </c>
       <c r="B102">
-        <v>0.89997629005364255</v>
+        <v>0.89726862616837721</v>
       </c>
       <c r="C102">
-        <v>58.399524802613627</v>
+        <v>44.506370065664527</v>
       </c>
       <c r="D102">
-        <v>0.60472879838903848</v>
+        <v>0.814289812903917</v>
       </c>
       <c r="E102">
-        <v>13.693234832829329</v>
+        <v>11.20779416912305</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>14.999951051812371</v>
+        <v>14.945063046250031</v>
       </c>
       <c r="B103">
-        <v>0.89710150977415848</v>
+        <v>0.55816606029487303</v>
       </c>
       <c r="C103">
-        <v>49.793898409180549</v>
+        <v>40.206530191785667</v>
       </c>
       <c r="D103">
-        <v>0.78197835791210779</v>
+        <v>0.90494318485091196</v>
       </c>
       <c r="E103">
-        <v>11.76650805569499</v>
+        <v>9.4467793005663943</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>14.99998550793147</v>
+        <v>14.945078838751179</v>
       </c>
       <c r="B104">
-        <v>0.37654615765144928</v>
+        <v>0.66529918753993877</v>
       </c>
       <c r="C104">
-        <v>40.008891497099647</v>
+        <v>40.263390217090461</v>
       </c>
       <c r="D104">
-        <v>0.91506076410740689</v>
+        <v>0.89492126307260267</v>
       </c>
       <c r="E104">
-        <v>8.5874391413424895</v>
+        <v>9.8942754468089316</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>14.999999999979391</v>
+        <v>14.94511630392064</v>
       </c>
       <c r="B105">
-        <v>0.87253226256897443</v>
+        <v>0.89409045073814741</v>
       </c>
       <c r="C105">
-        <v>45.033432551764633</v>
+        <v>59.538575326913637</v>
       </c>
       <c r="D105">
-        <v>0.81759684670387656</v>
+        <v>0.57565300348798132</v>
       </c>
       <c r="E105">
-        <v>11.209226757849169</v>
+        <v>13.811935253219129</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>14.998161778647569</v>
+        <v>14.94511802767021</v>
       </c>
       <c r="B106">
-        <v>0.8890199856113209</v>
+        <v>0.88148562687868326</v>
       </c>
       <c r="C106">
-        <v>52.258800289776723</v>
+        <v>50.970318740983657</v>
       </c>
       <c r="D106">
-        <v>0.7431299345563035</v>
+        <v>0.76818511586324867</v>
       </c>
       <c r="E106">
-        <v>12.290404488394261</v>
+        <v>11.93967402906314</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>14.999999417237539</v>
+        <v>14.94510827546733</v>
       </c>
       <c r="B107">
-        <v>0.84834653049442688</v>
+        <v>0.56589565759124949</v>
       </c>
       <c r="C107">
-        <v>44.373377667369759</v>
+        <v>40.19140270773616</v>
       </c>
       <c r="D107">
-        <v>0.82923464834308358</v>
+        <v>0.90435855096677509</v>
       </c>
       <c r="E107">
-        <v>11.055645171008351</v>
+        <v>9.4814756829499185</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>14.973195936395269</v>
+        <v>14.94511648655781</v>
       </c>
       <c r="B108">
-        <v>0.89991051393105437</v>
+        <v>0.89593561084325346</v>
       </c>
       <c r="C108">
-        <v>53.639951069335481</v>
+        <v>52.587450930885169</v>
       </c>
       <c r="D108">
-        <v>0.70589203527136057</v>
+        <v>0.73340446973542739</v>
       </c>
       <c r="E108">
-        <v>12.68480454815653</v>
+        <v>12.378593229098531</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>14.99999998671472</v>
+        <v>14.94510463406994</v>
       </c>
       <c r="B109">
-        <v>0.59660602559869069</v>
+        <v>0.89675258280679349</v>
       </c>
       <c r="C109">
-        <v>40.041099184823743</v>
+        <v>51.713177582554657</v>
       </c>
       <c r="D109">
-        <v>0.90255177978749412</v>
+        <v>0.75294322575849559</v>
       </c>
       <c r="E109">
-        <v>9.6347405592151834</v>
+        <v>12.15509094125111</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>14.99999999797684</v>
+        <v>14.94511753911554</v>
       </c>
       <c r="B110">
-        <v>0.78343392307876036</v>
+        <v>0.81326246039970052</v>
       </c>
       <c r="C110">
-        <v>56.555926589737673</v>
+        <v>57.157969681445493</v>
       </c>
       <c r="D110">
-        <v>0.69686190092412492</v>
+        <v>0.67446048571948614</v>
       </c>
       <c r="E110">
-        <v>12.81767764571169</v>
+        <v>13.064320779963269</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>14.999971132591281</v>
+        <v>14.9451161110321</v>
       </c>
       <c r="B111">
-        <v>0.84975678605971205</v>
+        <v>0.89747052946678096</v>
       </c>
       <c r="C111">
-        <v>49.995873115134117</v>
+        <v>53.127739332439617</v>
       </c>
       <c r="D111">
-        <v>0.78487409498513416</v>
+        <v>0.71944738841852551</v>
       </c>
       <c r="E111">
-        <v>11.678993801697599</v>
+        <v>12.52829097984479</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>14.9999978484278</v>
+        <v>14.94511847962097</v>
       </c>
       <c r="B112">
-        <v>0.85137058203565574</v>
+        <v>0.70172392728886612</v>
       </c>
       <c r="C112">
-        <v>43.384375512195192</v>
+        <v>40.191931934541913</v>
       </c>
       <c r="D112">
-        <v>0.8379776253776976</v>
+        <v>0.89103976393542106</v>
       </c>
       <c r="E112">
-        <v>10.936504152437379</v>
+        <v>10.01935021730195</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>14.999999998398749</v>
+        <v>14.94511623104014</v>
       </c>
       <c r="B113">
-        <v>0.70708441736403216</v>
+        <v>0.58024309044090117</v>
       </c>
       <c r="C113">
-        <v>40.035413457313112</v>
+        <v>40.361769086241488</v>
       </c>
       <c r="D113">
-        <v>0.89111422655434036</v>
+        <v>0.90252458333170593</v>
       </c>
       <c r="E113">
-        <v>10.05649116388169</v>
+        <v>9.5519576664973496</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>14.999999985816469</v>
+        <v>14.945115194961829</v>
       </c>
       <c r="B114">
-        <v>0.82691004075329388</v>
+        <v>0.79086319387048853</v>
       </c>
       <c r="C114">
-        <v>56.605627584993911</v>
+        <v>55.859222925325682</v>
       </c>
       <c r="D114">
-        <v>0.67939978442906079</v>
+        <v>0.70216421943546903</v>
       </c>
       <c r="E114">
-        <v>13.04557550883346</v>
+        <v>12.690745149914671</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>14.999866055701959</v>
+        <v>14.94511849731335</v>
       </c>
       <c r="B115">
-        <v>0.88204118248815355</v>
+        <v>0.48324940194454502</v>
       </c>
       <c r="C115">
-        <v>58.271136307118411</v>
+        <v>40.190298526193367</v>
       </c>
       <c r="D115">
-        <v>0.61811998780296151</v>
+        <v>0.91049399857125235</v>
       </c>
       <c r="E115">
-        <v>13.599796270928049</v>
+        <v>9.0894380734472744</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>14.99994945703806</v>
+        <v>14.94511728666674</v>
       </c>
       <c r="B116">
-        <v>0.61045183898550348</v>
+        <v>0.89710702608967197</v>
       </c>
       <c r="C116">
-        <v>40.02699181804077</v>
+        <v>58.116025530938657</v>
       </c>
       <c r="D116">
-        <v>0.90133743681287115</v>
+        <v>0.61087861783095332</v>
       </c>
       <c r="E116">
-        <v>9.6932957236302766</v>
+        <v>13.62641565769572</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>14.999987585468659</v>
+        <v>14.94511539308283</v>
       </c>
       <c r="B117">
-        <v>0.86496720333007715</v>
+        <v>0.80451554266693548</v>
       </c>
       <c r="C117">
-        <v>47.766797263662802</v>
+        <v>41.007998069960728</v>
       </c>
       <c r="D117">
-        <v>0.80186274589531992</v>
+        <v>0.87184166822429132</v>
       </c>
       <c r="E117">
-        <v>11.42562570163282</v>
+        <v>10.41746352692468</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>14.99998547415103</v>
+        <v>14.945118318753369</v>
       </c>
       <c r="B118">
-        <v>0.64889804940910345</v>
+        <v>0.592955334656314</v>
       </c>
       <c r="C118">
-        <v>40.026435572480828</v>
+        <v>40.191051536404032</v>
       </c>
       <c r="D118">
-        <v>0.89764418786681155</v>
+        <v>0.90206079806902151</v>
       </c>
       <c r="E118">
-        <v>9.8478963074470549</v>
+        <v>9.6010979677315653</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>14.99999933322723</v>
+        <v>14.94424418508415</v>
       </c>
       <c r="B119">
-        <v>0.89995597405704975</v>
+        <v>0.89687637699984102</v>
       </c>
       <c r="C119">
-        <v>52.637083766850303</v>
+        <v>53.333619483668507</v>
       </c>
       <c r="D119">
-        <v>0.73217216725383549</v>
+        <v>0.71424514656650551</v>
       </c>
       <c r="E119">
-        <v>12.42366669093807</v>
+        <v>12.58134978500718</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>14.999989668787901</v>
+        <v>14.945064520097709</v>
       </c>
       <c r="B120">
-        <v>0.88439428887483595</v>
+        <v>0.55022007145396479</v>
       </c>
       <c r="C120">
-        <v>46.564788765601243</v>
+        <v>40.19186475124387</v>
       </c>
       <c r="D120">
-        <v>0.8048836735992283</v>
+        <v>0.90562822792514608</v>
       </c>
       <c r="E120">
-        <v>11.379298477185939</v>
+        <v>9.4097625057662615</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>14.99999999970364</v>
+        <v>14.945116028930959</v>
       </c>
       <c r="B121">
-        <v>0.89489664955458836</v>
+        <v>0.89247253153476425</v>
       </c>
       <c r="C121">
-        <v>58.060853106714049</v>
+        <v>57.323619674757794</v>
       </c>
       <c r="D121">
-        <v>0.61555511148638054</v>
+        <v>0.63031442912480173</v>
       </c>
       <c r="E121">
-        <v>13.622029925413431</v>
+        <v>13.474632849089771</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>14.999999999648111</v>
+        <v>14.94511164985871</v>
       </c>
       <c r="B122">
-        <v>0.89724460506008885</v>
+        <v>0.8126195889099227</v>
       </c>
       <c r="C122">
-        <v>57.798317292143217</v>
+        <v>55.440872710982887</v>
       </c>
       <c r="D122">
-        <v>0.6198130528393665</v>
+        <v>0.69999886856996485</v>
       </c>
       <c r="E122">
-        <v>13.591289234227251</v>
+        <v>12.715906946652151</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>14.998150938021791</v>
+        <v>14.944785377793879</v>
       </c>
       <c r="B123">
-        <v>0.43911113596126933</v>
+        <v>0.85014665233782893</v>
       </c>
       <c r="C123">
-        <v>40.000206748502492</v>
+        <v>44.894808980421253</v>
       </c>
       <c r="D123">
-        <v>0.91348062864191049</v>
+        <v>0.82417220711216943</v>
       </c>
       <c r="E123">
-        <v>8.8822630837890806</v>
+        <v>11.09590669351863</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>14.99999669987656</v>
+        <v>14.94511850359601</v>
       </c>
       <c r="B124">
-        <v>0.88984828281015915</v>
+        <v>0.89631456042192581</v>
       </c>
       <c r="C124">
-        <v>50.954403724375872</v>
+        <v>51.796023782269494</v>
       </c>
       <c r="D124">
-        <v>0.76813078188442785</v>
+        <v>0.75130580960743309</v>
       </c>
       <c r="E124">
-        <v>11.977209024621359</v>
+        <v>12.174577450886661</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>14.999949129805771</v>
+        <v>14.94480426351481</v>
       </c>
       <c r="B125">
-        <v>0.8235746397116861</v>
+        <v>0.79641150088372503</v>
       </c>
       <c r="C125">
-        <v>40.993667295281021</v>
+        <v>41.798881531018282</v>
       </c>
       <c r="D125">
-        <v>0.86863526573510197</v>
+        <v>0.86631085217727855</v>
       </c>
       <c r="E125">
-        <v>10.502823014854769</v>
+        <v>10.494173040684711</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>14.99999841198211</v>
+        <v>14.94477883110088</v>
       </c>
       <c r="B126">
-        <v>0.89958169100586738</v>
+        <v>0.84205633274471403</v>
       </c>
       <c r="C126">
-        <v>50.350584600645469</v>
+        <v>45.469231653282293</v>
       </c>
       <c r="D126">
-        <v>0.77554169837891651</v>
+        <v>0.82188204713245605</v>
       </c>
       <c r="E126">
-        <v>11.87444355136739</v>
+        <v>11.127939796513269</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>14.999999999648111</v>
+        <v>14.94511790722397</v>
       </c>
       <c r="B127">
-        <v>0.89965712051049052</v>
+        <v>0.89704034851966474</v>
       </c>
       <c r="C127">
-        <v>58.341928928235319</v>
+        <v>49.912762403417602</v>
       </c>
       <c r="D127">
-        <v>0.60627410232597467</v>
+        <v>0.78012389826731288</v>
       </c>
       <c r="E127">
-        <v>13.6837179502424</v>
+        <v>11.76843540571627</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>14.99999999946586</v>
+        <v>14.94510738197391</v>
       </c>
       <c r="B128">
-        <v>0.8912518321908236</v>
+        <v>0.87625777142470951</v>
       </c>
       <c r="C128">
-        <v>51.523065438352141</v>
+        <v>50.096897206233777</v>
       </c>
       <c r="D128">
-        <v>0.75811966267340769</v>
+        <v>0.78040695073047395</v>
       </c>
       <c r="E128">
-        <v>12.112721931054169</v>
+        <v>11.74988860953184</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>14.999999999464441</v>
+        <v>14.945116306177461</v>
       </c>
       <c r="B129">
-        <v>0.89177070874759723</v>
+        <v>0.87355066446431118</v>
       </c>
       <c r="C129">
-        <v>51.447114381435739</v>
+        <v>44.673870357573954</v>
       </c>
       <c r="D129">
-        <v>0.75947444119369678</v>
+        <v>0.81973435229523361</v>
       </c>
       <c r="E129">
-        <v>12.09583767335841</v>
+        <v>11.149704079020619</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>14.99990741291632</v>
+        <v>14.9451184964764</v>
       </c>
       <c r="B130">
-        <v>0.89229496469828584</v>
+        <v>0.65340952379036688</v>
       </c>
       <c r="C130">
-        <v>56.93173364628138</v>
+        <v>40.200107344744097</v>
       </c>
       <c r="D130">
-        <v>0.63970290994556334</v>
+        <v>0.89634757333187931</v>
       </c>
       <c r="E130">
-        <v>13.420518714340041</v>
+        <v>9.8467406488625002</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>14.998954887110351</v>
+        <v>14.94510697907727</v>
       </c>
       <c r="B131">
-        <v>0.89773511871248701</v>
+        <v>0.89735178711265562</v>
       </c>
       <c r="C131">
-        <v>53.20155831250046</v>
+        <v>52.049402692974773</v>
       </c>
       <c r="D131">
-        <v>0.71835347768829427</v>
+        <v>0.74570598848998393</v>
       </c>
       <c r="E131">
-        <v>12.568497201056029</v>
+        <v>12.24187092486579</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>14.999988955705859</v>
+        <v>14.944765483607521</v>
       </c>
       <c r="B132">
-        <v>0.88927278881316774</v>
+        <v>0.89754279042873153</v>
       </c>
       <c r="C132">
-        <v>47.761867477695617</v>
+        <v>57.996503936092303</v>
       </c>
       <c r="D132">
-        <v>0.79739228508465565</v>
+        <v>0.61326923168000003</v>
       </c>
       <c r="E132">
-        <v>11.49095843531002</v>
+        <v>13.609604035992509</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>14.99999968523287</v>
+        <v>14.94511599120151</v>
       </c>
       <c r="B133">
-        <v>0.89955794697131886</v>
+        <v>0.89062047853608839</v>
       </c>
       <c r="C133">
-        <v>59.866020748996917</v>
+        <v>53.669644269520212</v>
       </c>
       <c r="D133">
-        <v>0.56627944095694271</v>
+        <v>0.70739024903580916</v>
       </c>
       <c r="E133">
-        <v>13.871550513926151</v>
+        <v>12.64870111557571</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>14.999980333555101</v>
+        <v>14.94511842482193</v>
       </c>
       <c r="B134">
-        <v>0.89937543870826475</v>
+        <v>0.8926047857196644</v>
       </c>
       <c r="C134">
-        <v>57.489657486122127</v>
+        <v>48.371147141048581</v>
       </c>
       <c r="D134">
-        <v>0.62477914855160277</v>
+        <v>0.79267337828587559</v>
       </c>
       <c r="E134">
-        <v>13.55055270357985</v>
+        <v>11.540715049454629</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>14.999789860655691</v>
+        <v>14.94511659019337</v>
       </c>
       <c r="B135">
-        <v>0.49033012016485938</v>
+        <v>0.89752880255676493</v>
       </c>
       <c r="C135">
-        <v>40.010225834441933</v>
+        <v>59.58312798772252</v>
       </c>
       <c r="D135">
-        <v>0.9107276601312726</v>
+        <v>0.57284839986237768</v>
       </c>
       <c r="E135">
-        <v>9.1359228146691933</v>
+        <v>13.82840767275168</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>14.99999186935767</v>
+        <v>14.94511848439201</v>
       </c>
       <c r="B136">
-        <v>0.84864277451111847</v>
+        <v>0.89561301686459227</v>
       </c>
       <c r="C136">
-        <v>46.197248934839408</v>
+        <v>41.270551650855182</v>
       </c>
       <c r="D136">
-        <v>0.8156774079811745</v>
+        <v>0.84919307390717724</v>
       </c>
       <c r="E136">
-        <v>11.23991715770873</v>
+        <v>10.72459448886576</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>14.9999978484278</v>
+        <v>14.945115872880271</v>
       </c>
       <c r="B137">
-        <v>0.876289077914988</v>
+        <v>0.82567632090582954</v>
       </c>
       <c r="C137">
-        <v>57.487937960966377</v>
+        <v>42.9109080685067</v>
       </c>
       <c r="D137">
-        <v>0.63866186527996838</v>
+        <v>0.84868808885365776</v>
       </c>
       <c r="E137">
-        <v>13.44560092850084</v>
+        <v>10.752888176071821</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>14.9987772237969</v>
+        <v>14.94511847311667</v>
       </c>
       <c r="B138">
-        <v>0.39940979490658007</v>
+        <v>0.84650118195544422</v>
       </c>
       <c r="C138">
-        <v>40.019076090941468</v>
+        <v>47.296272079354253</v>
       </c>
       <c r="D138">
-        <v>0.91476039715047786</v>
+        <v>0.80796963063519478</v>
       </c>
       <c r="E138">
-        <v>8.6921895137610186</v>
+        <v>11.30667092666345</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>14.999999322451711</v>
+        <v>14.936239148191451</v>
       </c>
       <c r="B139">
-        <v>0.86542455310856425</v>
+        <v>0.81562641266656055</v>
       </c>
       <c r="C139">
-        <v>46.248349188304857</v>
+        <v>56.650486237122927</v>
       </c>
       <c r="D139">
-        <v>0.811374725758222</v>
+        <v>0.68173190393645366</v>
       </c>
       <c r="E139">
-        <v>11.297095134690061</v>
+        <v>12.97159285274522</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>14.99999960155847</v>
+        <v>14.945117903640361</v>
       </c>
       <c r="B140">
-        <v>0.88314222411106302</v>
+        <v>0.8969012594432213</v>
       </c>
       <c r="C140">
-        <v>51.447114381435739</v>
+        <v>58.173777107654892</v>
       </c>
       <c r="D140">
-        <v>0.76058466173639794</v>
+        <v>0.60968796668665981</v>
       </c>
       <c r="E140">
-        <v>12.072468130105509</v>
+        <v>13.63440986697646</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>14.99999998541522</v>
+        <v>14.945118368603611</v>
       </c>
       <c r="B141">
-        <v>0.89310072998732493</v>
+        <v>0.86995590615345919</v>
       </c>
       <c r="C141">
-        <v>47.064913496523559</v>
+        <v>47.722284200893156</v>
       </c>
       <c r="D141">
-        <v>0.80020023071516444</v>
+        <v>0.80064351092197994</v>
       </c>
       <c r="E141">
-        <v>11.44265297695693</v>
+        <v>11.415056749823471</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>14.99999907810769</v>
+        <v>14.945084935947859</v>
       </c>
       <c r="B142">
-        <v>0.89995597405704975</v>
+        <v>0.710185313453222</v>
       </c>
       <c r="C142">
-        <v>48.446782232605287</v>
+        <v>40.243744743471389</v>
       </c>
       <c r="D142">
-        <v>0.7916938244319639</v>
+        <v>0.88987148629421819</v>
       </c>
       <c r="E142">
-        <v>11.58592976942993</v>
+        <v>10.05071975092104</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>14.999999606720451</v>
+        <v>14.945118318753369</v>
       </c>
       <c r="B143">
-        <v>0.89567002664103457</v>
+        <v>0.60311285565817374</v>
       </c>
       <c r="C143">
-        <v>58.253765585807969</v>
+        <v>40.191051536404032</v>
       </c>
       <c r="D143">
-        <v>0.61069641361823046</v>
+        <v>0.90116250459588221</v>
       </c>
       <c r="E143">
-        <v>13.6543377031005</v>
+        <v>9.6445078458432221</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>14.99994234633405</v>
+        <v>14.945084935947859</v>
       </c>
       <c r="B144">
-        <v>0.89282538329782157</v>
+        <v>0.41194469882364992</v>
       </c>
       <c r="C144">
-        <v>58.697814704835586</v>
+        <v>40.243744743471389</v>
       </c>
       <c r="D144">
-        <v>0.60144905888015454</v>
+        <v>0.91397754840121259</v>
       </c>
       <c r="E144">
-        <v>13.706496853851529</v>
+        <v>8.7467657758025368</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>14.99999996216822</v>
+        <v>14.943166505880979</v>
       </c>
       <c r="B145">
-        <v>0.89736175061480972</v>
+        <v>0.897550016203707</v>
       </c>
       <c r="C145">
-        <v>58.779186864573781</v>
+        <v>53.262140041245061</v>
       </c>
       <c r="D145">
-        <v>0.5968633430224648</v>
+        <v>0.7159088820814159</v>
       </c>
       <c r="E145">
-        <v>13.73514231651232</v>
+        <v>12.56404925223632</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>14.99999999972631</v>
+        <v>14.94511848625921</v>
       </c>
       <c r="B146">
-        <v>0.57961601996406908</v>
+        <v>0.47165857243961318</v>
       </c>
       <c r="C146">
-        <v>40.023094987601617</v>
+        <v>40.211575119713537</v>
       </c>
       <c r="D146">
-        <v>0.90405000520358725</v>
+        <v>0.91116056405079471</v>
       </c>
       <c r="E146">
-        <v>9.5596701018412844</v>
+        <v>9.0334872161650228</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>14.999999914241791</v>
+        <v>14.94511728349608</v>
       </c>
       <c r="B147">
-        <v>0.89421992350903556</v>
+        <v>0.69589608095048983</v>
       </c>
       <c r="C147">
-        <v>53.311038634401378</v>
+        <v>40.192222563163227</v>
       </c>
       <c r="D147">
-        <v>0.71646776307827187</v>
+        <v>0.89173116129293128</v>
       </c>
       <c r="E147">
-        <v>12.58645124930834</v>
+        <v>9.9995485883956494</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>14.999999988461621</v>
+        <v>14.94449871402295</v>
       </c>
       <c r="B148">
-        <v>0.68172635107617341</v>
+        <v>0.79086319387048853</v>
       </c>
       <c r="C148">
-        <v>40.266558388994703</v>
+        <v>56.1822679351462</v>
       </c>
       <c r="D148">
-        <v>0.89357878468552721</v>
+        <v>0.69803156737108718</v>
       </c>
       <c r="E148">
-        <v>9.9809361353258943</v>
+        <v>12.75553441348613</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>14.99999999638675</v>
+        <v>14.940200190180709</v>
       </c>
       <c r="B149">
-        <v>0.85078441346185141</v>
+        <v>0.79896738812483559</v>
       </c>
       <c r="C149">
-        <v>41.949636658703021</v>
+        <v>55.906653079904707</v>
       </c>
       <c r="D149">
-        <v>0.85400630713379055</v>
+        <v>0.69864894071716876</v>
       </c>
       <c r="E149">
-        <v>10.72092850293676</v>
+        <v>12.73964156705205</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>14.99999907810769</v>
+        <v>14.94338119898284</v>
       </c>
       <c r="B150">
-        <v>0.89995597405704975</v>
+        <v>0.897550016203707</v>
       </c>
       <c r="C150">
-        <v>52.705071688095693</v>
+        <v>53.4813778015792</v>
       </c>
       <c r="D150">
-        <v>0.73048472129643238</v>
+        <v>0.7101934511293172</v>
       </c>
       <c r="E150">
-        <v>12.441942742130021</v>
+        <v>12.62306398620254</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>14.999999997981581</v>
+        <v>14.94511842482193</v>
       </c>
       <c r="B151">
-        <v>0.89829975257869477</v>
+        <v>0.8926047857196644</v>
       </c>
       <c r="C151">
-        <v>46.313117161815043</v>
+        <v>49.502038943922138</v>
       </c>
       <c r="D151">
-        <v>0.80265079057578681</v>
+        <v>0.78454111590360454</v>
       </c>
       <c r="E151">
-        <v>11.399727975776811</v>
+        <v>11.689685539392951</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>14.999960229344611</v>
+        <v>14.94511849790616</v>
       </c>
       <c r="B152">
-        <v>0.84262787233791403</v>
+        <v>0.84933840947093919</v>
       </c>
       <c r="C152">
-        <v>40.697295074488139</v>
+        <v>57.464067625480993</v>
       </c>
       <c r="D152">
-        <v>0.86651680670272213</v>
+        <v>0.65184188886506544</v>
       </c>
       <c r="E152">
-        <v>10.52085642051132</v>
+        <v>13.29727570971688</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>14.99872208092866</v>
+        <v>14.945116526581369</v>
       </c>
       <c r="B153">
-        <v>0.41876607727542808</v>
+        <v>0.85024979643322884</v>
       </c>
       <c r="C153">
-        <v>40.015428294086853</v>
+        <v>42.008286207363341</v>
       </c>
       <c r="D153">
-        <v>0.91424317968255531</v>
+        <v>0.85321186573822705</v>
       </c>
       <c r="E153">
-        <v>8.7839460135635186</v>
+        <v>10.69895891527508</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>14.999509610174551</v>
+        <v>14.940801570564091</v>
       </c>
       <c r="B154">
-        <v>0.87668352423280449</v>
+        <v>0.89322146699662275</v>
       </c>
       <c r="C154">
-        <v>58.135442097593099</v>
+        <v>51.98993195403672</v>
       </c>
       <c r="D154">
-        <v>0.6243412828601097</v>
+        <v>0.74761323630471166</v>
       </c>
       <c r="E154">
-        <v>13.55544919678475</v>
+        <v>12.213312494553319</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>14.9999978484278</v>
+        <v>14.945116239018789</v>
       </c>
       <c r="B155">
-        <v>0.85137058203565574</v>
+        <v>0.83215715139843416</v>
       </c>
       <c r="C155">
-        <v>42.444566616785082</v>
+        <v>42.206516228452422</v>
       </c>
       <c r="D155">
-        <v>0.84838755384289066</v>
+        <v>0.8550628161240118</v>
       </c>
       <c r="E155">
-        <v>10.797859495961831</v>
+        <v>10.67022244963338</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>14.99999989751014</v>
+        <v>14.945108330713561</v>
       </c>
       <c r="B156">
-        <v>0.84821904926453462</v>
+        <v>0.89755268433696322</v>
       </c>
       <c r="C156">
-        <v>57.277719924336857</v>
+        <v>53.510265498274897</v>
       </c>
       <c r="D156">
-        <v>0.65790027208478763</v>
+        <v>0.70946865083005661</v>
       </c>
       <c r="E156">
-        <v>13.277147649478779</v>
+        <v>12.631449514587059</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>14.999999992977351</v>
+        <v>14.945118500682261</v>
       </c>
       <c r="B157">
-        <v>0.89944107407506724</v>
+        <v>0.84114114266012274</v>
       </c>
       <c r="C157">
-        <v>47.694310563126358</v>
+        <v>40.561102381982089</v>
       </c>
       <c r="D157">
-        <v>0.79573968898405512</v>
+        <v>0.86717004409299747</v>
       </c>
       <c r="E157">
-        <v>11.51096828926392</v>
+        <v>10.470383049725131</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>14.99999995494033</v>
+        <v>14.94508723518444</v>
       </c>
       <c r="B158">
-        <v>0.56961187362357091</v>
+        <v>0.53445316363549888</v>
       </c>
       <c r="C158">
-        <v>40.027374092387873</v>
+        <v>40.284025388943952</v>
       </c>
       <c r="D158">
-        <v>0.90487648822554867</v>
+        <v>0.90655366228535161</v>
       </c>
       <c r="E158">
-        <v>9.5147676824808975</v>
+        <v>9.3391137903188852</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>14.99999970584463</v>
+        <v>14.944257007770251</v>
       </c>
       <c r="B159">
-        <v>0.72975773142023703</v>
+        <v>0.88681416066231</v>
       </c>
       <c r="C159">
-        <v>40.531304364952518</v>
+        <v>53.757885309240343</v>
       </c>
       <c r="D159">
-        <v>0.88670779455325588</v>
+        <v>0.70630854393018494</v>
       </c>
       <c r="E159">
-        <v>10.16410263607715</v>
+        <v>12.65724571030497</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>14.99999886882261</v>
+        <v>14.945118425366511</v>
       </c>
       <c r="B160">
-        <v>0.89995597405704975</v>
+        <v>0.79481970640801758</v>
       </c>
       <c r="C160">
-        <v>51.046001839420427</v>
+        <v>41.402388308635118</v>
       </c>
       <c r="D160">
-        <v>0.76548523536651503</v>
+        <v>0.87037789598601123</v>
       </c>
       <c r="E160">
-        <v>12.023045775694129</v>
+        <v>10.436510928165831</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>14.99999996220081</v>
+        <v>14.94511761086804</v>
       </c>
       <c r="B161">
-        <v>0.89082292528526885</v>
+        <v>0.88307673397789854</v>
       </c>
       <c r="C161">
-        <v>53.80057050011839</v>
+        <v>48.967093821886529</v>
       </c>
       <c r="D161">
-        <v>0.70504766875469338</v>
+        <v>0.79007582754672256</v>
       </c>
       <c r="E161">
-        <v>12.70424654252472</v>
+        <v>11.58893493344428</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>14.999999261958481</v>
+        <v>14.94511838733499</v>
       </c>
       <c r="B162">
-        <v>0.86284154984228811</v>
+        <v>0.80881994880864316</v>
       </c>
       <c r="C162">
-        <v>47.036904715666452</v>
+        <v>46.337284040489443</v>
       </c>
       <c r="D162">
-        <v>0.80701985547534738</v>
+        <v>0.82273175634455964</v>
       </c>
       <c r="E162">
-        <v>11.35456594234806</v>
+        <v>11.09593123507633</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>14.99999997175531</v>
+        <v>14.94511785868951</v>
       </c>
       <c r="B163">
-        <v>0.83465311058392289</v>
+        <v>0.52823393395108353</v>
       </c>
       <c r="C163">
-        <v>41.002088002756857</v>
+        <v>40.19959164975559</v>
       </c>
       <c r="D163">
-        <v>0.86629715694894194</v>
+        <v>0.90731138410785095</v>
       </c>
       <c r="E163">
-        <v>10.536678637557481</v>
+        <v>9.3069250477630483</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>14.99999999797565</v>
+        <v>14.94511848982156</v>
       </c>
       <c r="B164">
-        <v>0.78822944927383765</v>
+        <v>0.89413769621784822</v>
       </c>
       <c r="C164">
-        <v>56.338633943230207</v>
+        <v>50.24346634002184</v>
       </c>
       <c r="D164">
-        <v>0.69824242850390728</v>
+        <v>0.77678078837141118</v>
       </c>
       <c r="E164">
-        <v>12.79835025796296</v>
+        <v>11.822174703068841</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>14.99999996220081</v>
+        <v>14.945116306177461</v>
       </c>
       <c r="B165">
-        <v>0.89641612148746697</v>
+        <v>0.86312598708299948</v>
       </c>
       <c r="C165">
-        <v>53.80057050011839</v>
+        <v>43.529282792980908</v>
       </c>
       <c r="D165">
-        <v>0.7033045341946158</v>
+        <v>0.83320688570682444</v>
       </c>
       <c r="E165">
-        <v>12.72480896453944</v>
+        <v>10.969406445242161</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>14.999998002718741</v>
+        <v>14.94511558977379</v>
       </c>
       <c r="B166">
-        <v>0.89995597405704975</v>
+        <v>0.85873498473390653</v>
       </c>
       <c r="C166">
-        <v>51.128207793547517</v>
+        <v>46.618139380803989</v>
       </c>
       <c r="D166">
-        <v>0.76411331388248604</v>
+        <v>0.81008071004265447</v>
       </c>
       <c r="E166">
-        <v>12.041855013310551</v>
+        <v>11.285329986325159</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>14.99999687866136</v>
+        <v>14.94511750578758</v>
       </c>
       <c r="B167">
-        <v>0.86344862105284048</v>
+        <v>0.84341075823079936</v>
       </c>
       <c r="C167">
-        <v>42.773698777039222</v>
+        <v>57.442536591602043</v>
       </c>
       <c r="D167">
-        <v>0.84170723493713273</v>
+        <v>0.65525174741460879</v>
       </c>
       <c r="E167">
-        <v>10.88729703343647</v>
+        <v>13.265126751644081</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>14.99999708164839</v>
+        <v>14.94511539308283</v>
       </c>
       <c r="B168">
-        <v>0.89141461374699438</v>
+        <v>0.66876363022971763</v>
       </c>
       <c r="C168">
-        <v>58.975709003208507</v>
+        <v>40.219420254391743</v>
       </c>
       <c r="D168">
-        <v>0.59485815749597204</v>
+        <v>0.89469168796001819</v>
       </c>
       <c r="E168">
-        <v>13.73905910945866</v>
+        <v>9.9048599394024972</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>14.999998572024779</v>
+        <v>14.944925276461211</v>
       </c>
       <c r="B169">
-        <v>0.89254608558813087</v>
+        <v>0.84203512036735617</v>
       </c>
       <c r="C169">
-        <v>41.976461552150838</v>
+        <v>44.894808980421253</v>
       </c>
       <c r="D169">
-        <v>0.84317045728060724</v>
+        <v>0.82619707984061408</v>
       </c>
       <c r="E169">
-        <v>10.855667426776259</v>
+        <v>11.068362947938949</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>14.99999448403049</v>
+        <v>14.945073705026051</v>
       </c>
       <c r="B170">
-        <v>0.78950874497563384</v>
+        <v>0.89710702608967197</v>
       </c>
       <c r="C170">
-        <v>40.537785949282629</v>
+        <v>57.683437458465967</v>
       </c>
       <c r="D170">
-        <v>0.87763257675471662</v>
+        <v>0.62023724015591131</v>
       </c>
       <c r="E170">
-        <v>10.350420470053351</v>
+        <v>13.55725696254234</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>14.999999989434251</v>
+        <v>14.944791714393819</v>
       </c>
       <c r="B171">
-        <v>0.67596472115927275</v>
+        <v>0.89069169980976548</v>
       </c>
       <c r="C171">
-        <v>40.035794177892711</v>
+        <v>49.693254026059961</v>
       </c>
       <c r="D171">
-        <v>0.89476170161780777</v>
+        <v>0.78301741366329547</v>
       </c>
       <c r="E171">
-        <v>9.9489161414255332</v>
+        <v>11.715708754361181</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>14.99999957889133</v>
+        <v>14.94511809466813</v>
       </c>
       <c r="B172">
-        <v>0.44409496403311211</v>
+        <v>0.49820550853360479</v>
       </c>
       <c r="C172">
-        <v>40.019074049696307</v>
+        <v>40.214145851956623</v>
       </c>
       <c r="D172">
-        <v>0.91325417077368187</v>
+        <v>0.90943461426392469</v>
       </c>
       <c r="E172">
-        <v>8.9076447943845469</v>
+        <v>9.1630209051799429</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>14.999999989434251</v>
+        <v>14.94511850560122</v>
       </c>
       <c r="B173">
-        <v>0.67324017696734184</v>
+        <v>0.4706779366160011</v>
       </c>
       <c r="C173">
-        <v>40.019414100409783</v>
+        <v>40.230937793671288</v>
       </c>
       <c r="D173">
-        <v>0.89508530823679333</v>
+        <v>0.91116721444307303</v>
       </c>
       <c r="E173">
-        <v>9.9384079701442154</v>
+        <v>9.0293399951143627</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>14.99984545476436</v>
+        <v>14.94511847875143</v>
       </c>
       <c r="B174">
-        <v>0.8608082137271813</v>
+        <v>0.7494194344330718</v>
       </c>
       <c r="C174">
-        <v>57.428210238473781</v>
+        <v>40.304222791190668</v>
       </c>
       <c r="D174">
-        <v>0.64843534311140338</v>
+        <v>0.88444461976778677</v>
       </c>
       <c r="E174">
-        <v>13.363588982639399</v>
+        <v>10.18008371695813</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>14.999999959490619</v>
+        <v>14.945118505848731</v>
       </c>
       <c r="B175">
-        <v>0.7943539530391972</v>
+        <v>0.897536691079585</v>
       </c>
       <c r="C175">
-        <v>56.569417415373529</v>
+        <v>59.875619038407777</v>
       </c>
       <c r="D175">
-        <v>0.69292565696484754</v>
+        <v>0.5646462592484055</v>
       </c>
       <c r="E175">
-        <v>12.875783794934881</v>
+        <v>13.861847752782619</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>14.999999959490619</v>
+        <v>14.94511650814991</v>
       </c>
       <c r="B176">
-        <v>0.79154880185655596</v>
+        <v>0.89734639647718295</v>
       </c>
       <c r="C176">
-        <v>56.559890064835997</v>
+        <v>51.933173004785893</v>
       </c>
       <c r="D176">
-        <v>0.69405336020686437</v>
+        <v>0.74824744274526234</v>
       </c>
       <c r="E176">
-        <v>12.859682188883699</v>
+        <v>12.2121075621599</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>14.999999999466951</v>
+        <v>14.945117980633061</v>
       </c>
       <c r="B177">
-        <v>0.89112093672765325</v>
+        <v>0.83236403787336699</v>
       </c>
       <c r="C177">
-        <v>48.08855984061433</v>
+        <v>41.312560489246628</v>
       </c>
       <c r="D177">
-        <v>0.79523461325233635</v>
+        <v>0.86398415298521036</v>
       </c>
       <c r="E177">
-        <v>11.52676561389565</v>
+        <v>10.541607323242941</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>14.99999954188063</v>
+        <v>14.945117348731779</v>
       </c>
       <c r="B178">
-        <v>0.89661478487058643</v>
+        <v>0.38813907354092092</v>
       </c>
       <c r="C178">
-        <v>58.583295897161364</v>
+        <v>40.190298332152757</v>
       </c>
       <c r="D178">
-        <v>0.60222480139129719</v>
+        <v>0.91469729949610212</v>
       </c>
       <c r="E178">
-        <v>13.70549345392403</v>
+        <v>8.6348952730735178</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>14.999980121912159</v>
+        <v>14.945118480911461</v>
       </c>
       <c r="B179">
-        <v>0.86492316311452722</v>
+        <v>0.64576879392851516</v>
       </c>
       <c r="C179">
-        <v>46.556885480630683</v>
+        <v>40.191931934541913</v>
       </c>
       <c r="D179">
-        <v>0.80957302009487708</v>
+        <v>0.89714053462548815</v>
       </c>
       <c r="E179">
-        <v>11.321030427173159</v>
+        <v>9.8171562024409926</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>14.999997232939361</v>
+        <v>14.945118167522921</v>
       </c>
       <c r="B180">
-        <v>0.73120706056933271</v>
+        <v>0.89537885913946158</v>
       </c>
       <c r="C180">
-        <v>40.266408800883568</v>
+        <v>51.033449498322163</v>
       </c>
       <c r="D180">
-        <v>0.8875218399490441</v>
+        <v>0.76556644637875504</v>
       </c>
       <c r="E180">
-        <v>10.14902402192306</v>
+        <v>11.99003950449651</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>14.998150938021791</v>
+        <v>14.944616728456509</v>
       </c>
       <c r="B181">
-        <v>0.40291595795166979</v>
+        <v>0.89465315033056281</v>
       </c>
       <c r="C181">
-        <v>40.010329318282778</v>
+        <v>58.977226200696293</v>
       </c>
       <c r="D181">
-        <v>0.91468364538970082</v>
+        <v>0.59092998342468273</v>
       </c>
       <c r="E181">
-        <v>8.7082482649069668</v>
+        <v>13.74119230788887</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>14.999985530504389</v>
+        <v>14.94511650814991</v>
       </c>
       <c r="B182">
-        <v>0.4296252479572587</v>
+        <v>0.89734639647718295</v>
       </c>
       <c r="C182">
-        <v>40.035941927202323</v>
+        <v>51.574845993015067</v>
       </c>
       <c r="D182">
-        <v>0.91384851748535501</v>
+        <v>0.75561778235269084</v>
       </c>
       <c r="E182">
-        <v>8.8373072941301789</v>
+        <v>12.122573695155401</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>14.99920813174351</v>
+        <v>14.9446809719062</v>
       </c>
       <c r="B183">
-        <v>0.85592428137472232</v>
+        <v>0.8686483795917419</v>
       </c>
       <c r="C183">
-        <v>47.036904715666452</v>
+        <v>58.512482609684618</v>
       </c>
       <c r="D183">
-        <v>0.80845237166316075</v>
+        <v>0.61701656527358351</v>
       </c>
       <c r="E183">
-        <v>11.33358198843907</v>
+        <v>13.568041230560629</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>14.999999721615531</v>
+        <v>14.94511835742477</v>
       </c>
       <c r="B184">
-        <v>0.47610161841794429</v>
+        <v>0.8832976554849572</v>
       </c>
       <c r="C184">
-        <v>40.004056354215962</v>
+        <v>46.318117186119473</v>
       </c>
       <c r="D184">
-        <v>0.91160068327671318</v>
+        <v>0.80600788860171546</v>
       </c>
       <c r="E184">
-        <v>9.06550281804906</v>
+        <v>11.335032366450889</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>14.9999997481289</v>
+        <v>14.94511845460327</v>
       </c>
       <c r="B185">
-        <v>0.47656554535142642</v>
+        <v>0.79195180318806835</v>
       </c>
       <c r="C185">
-        <v>40.173374854419507</v>
+        <v>40.909552728885558</v>
       </c>
       <c r="D185">
-        <v>0.91127010372227368</v>
+        <v>0.87475772899099691</v>
       </c>
       <c r="E185">
-        <v>9.0721857302820297</v>
+        <v>10.36767650297743</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>14.9999978484278</v>
+        <v>14.944802774443181</v>
       </c>
       <c r="B186">
-        <v>0.876289077914988</v>
+        <v>0.84987383605953837</v>
       </c>
       <c r="C186">
-        <v>57.204019117322893</v>
+        <v>57.062368715075579</v>
       </c>
       <c r="D186">
-        <v>0.64412779231551764</v>
+        <v>0.65920510531456467</v>
       </c>
       <c r="E186">
-        <v>13.39554268451162</v>
+        <v>13.22433277577885</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>14.99994234633405</v>
+        <v>14.94511715560501</v>
       </c>
       <c r="B187">
-        <v>0.87888719366376888</v>
+        <v>0.89679357388315706</v>
       </c>
       <c r="C187">
-        <v>58.433377881058803</v>
+        <v>57.745600547454053</v>
       </c>
       <c r="D187">
-        <v>0.61582602111606621</v>
+        <v>0.6191377806829268</v>
       </c>
       <c r="E187">
-        <v>13.61182170923594</v>
+        <v>13.566083845488951</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>14.99999964676276</v>
+        <v>14.944791714393819</v>
       </c>
       <c r="B188">
-        <v>0.83269256230910105</v>
+        <v>0.89575873873249112</v>
       </c>
       <c r="C188">
-        <v>43.018892525182942</v>
+        <v>49.693254026059961</v>
       </c>
       <c r="D188">
-        <v>0.84626446151042067</v>
+        <v>0.78242802702472547</v>
       </c>
       <c r="E188">
-        <v>10.820834151573919</v>
+        <v>11.72785330363709</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>14.999998337439161</v>
+        <v>14.94511848932914</v>
       </c>
       <c r="B189">
-        <v>0.89993415666438015</v>
+        <v>0.51812742709678816</v>
       </c>
       <c r="C189">
-        <v>50.986026411635358</v>
+        <v>40.205560194057561</v>
       </c>
       <c r="D189">
-        <v>0.7664630230924192</v>
+        <v>0.90804531195288918</v>
       </c>
       <c r="E189">
-        <v>12.00943813141952</v>
+        <v>9.2589005638937039</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>14.999999999979391</v>
+        <v>14.945118505814531</v>
       </c>
       <c r="B190">
-        <v>0.87356011390366661</v>
+        <v>0.81676787415506302</v>
       </c>
       <c r="C190">
-        <v>45.158333874731149</v>
+        <v>56.220427228714769</v>
       </c>
       <c r="D190">
-        <v>0.81641112721688569</v>
+        <v>0.68778243759226276</v>
       </c>
       <c r="E190">
-        <v>11.225069023463931</v>
+        <v>12.89534322060973</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>14.99999991133328</v>
+        <v>14.944855552554539</v>
       </c>
       <c r="B191">
-        <v>0.82663223395317331</v>
+        <v>0.89559230014594282</v>
       </c>
       <c r="C191">
-        <v>40.718955638567998</v>
+        <v>52.705081552246277</v>
       </c>
       <c r="D191">
-        <v>0.86976619090570573</v>
+        <v>0.73058240715583977</v>
       </c>
       <c r="E191">
-        <v>10.478022459550781</v>
+        <v>12.40872375264038</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>14.999999502036269</v>
+        <v>14.945111962226729</v>
       </c>
       <c r="B192">
-        <v>0.5957695089503684</v>
+        <v>0.8842996621905459</v>
       </c>
       <c r="C192">
-        <v>40.041099184823743</v>
+        <v>48.815308341994779</v>
       </c>
       <c r="D192">
-        <v>0.90262531451709027</v>
+        <v>0.79102241359459347</v>
       </c>
       <c r="E192">
-        <v>9.6311230834540567</v>
+        <v>11.57227643275561</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>14.99998811562798</v>
+        <v>14.945109659014481</v>
       </c>
       <c r="B193">
-        <v>0.87838595367461381</v>
+        <v>0.81745732990469999</v>
       </c>
       <c r="C193">
-        <v>47.766797263662802</v>
+        <v>56.650486237122927</v>
       </c>
       <c r="D193">
-        <v>0.79942136103811701</v>
+        <v>0.68121548876551508</v>
       </c>
       <c r="E193">
-        <v>11.462600340352409</v>
+        <v>12.984503870150659</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>14.999987585468659</v>
+        <v>14.944785377793879</v>
       </c>
       <c r="B194">
-        <v>0.88336749334568776</v>
+        <v>0.842518706061823</v>
       </c>
       <c r="C194">
-        <v>47.766797263662802</v>
+        <v>44.894808980421253</v>
       </c>
       <c r="D194">
-        <v>0.79848899480676461</v>
+        <v>0.82607723221693774</v>
       </c>
       <c r="E194">
-        <v>11.4759129155577</v>
+        <v>11.06995422980013</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>14.9999999992162</v>
+        <v>14.94449871402295</v>
       </c>
       <c r="B195">
-        <v>0.89493180003461792</v>
+        <v>0.79086319387048853</v>
       </c>
       <c r="C195">
-        <v>57.766845528643067</v>
+        <v>55.924191297070649</v>
       </c>
       <c r="D195">
-        <v>0.62189224251653374</v>
+        <v>0.70133487264351879</v>
       </c>
       <c r="E195">
-        <v>13.576083795984299</v>
+        <v>12.7035631647143</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>14.999999990535301</v>
+        <v>14.94511844683395</v>
       </c>
       <c r="B196">
-        <v>0.8509487224557839</v>
+        <v>0.86910629305587239</v>
       </c>
       <c r="C196">
-        <v>57.636229403598954</v>
+        <v>43.711986247580263</v>
       </c>
       <c r="D196">
-        <v>0.64933187676701898</v>
+        <v>0.8297474616123196</v>
       </c>
       <c r="E196">
-        <v>13.355468366322111</v>
+        <v>11.01483270528662</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>14.99999833526911</v>
+        <v>14.94511848870005</v>
       </c>
       <c r="B197">
-        <v>0.89993415666438015</v>
+        <v>0.37549469034017968</v>
       </c>
       <c r="C197">
-        <v>50.918038490389968</v>
+        <v>40.214419530320697</v>
       </c>
       <c r="D197">
-        <v>0.76754243674918876</v>
+        <v>0.9148438457441701</v>
       </c>
       <c r="E197">
-        <v>11.99424975845854</v>
+        <v>8.5796454894737515</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>14.99964211018332</v>
+        <v>14.945118154492601</v>
       </c>
       <c r="B198">
-        <v>0.57408809024703944</v>
+        <v>0.59481500184325531</v>
       </c>
       <c r="C198">
-        <v>40.000006536365149</v>
+        <v>40.324528023468773</v>
       </c>
       <c r="D198">
-        <v>0.90455040608249071</v>
+        <v>0.90142212268390254</v>
       </c>
       <c r="E198">
-        <v>9.5342156416549635</v>
+        <v>9.6141658633342235</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>14.99999997961344</v>
+        <v>14.945108724447829</v>
       </c>
       <c r="B199">
-        <v>0.83899985132975541</v>
+        <v>0.80163083904315025</v>
       </c>
       <c r="C199">
-        <v>41.417476838033657</v>
+        <v>41.444557501187766</v>
       </c>
       <c r="D199">
-        <v>0.86195949692538043</v>
+        <v>0.86878807421071036</v>
       </c>
       <c r="E199">
-        <v>10.60623066807541</v>
+        <v>10.46368375817134</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>14.999999928521291</v>
+        <v>14.9451184867157</v>
       </c>
       <c r="B200">
-        <v>0.79532851835294649</v>
+        <v>0.89675258280679349</v>
       </c>
       <c r="C200">
-        <v>40.718955638567998</v>
+        <v>51.210002835947783</v>
       </c>
       <c r="D200">
-        <v>0.87570641590677456</v>
+        <v>0.7624310724505754</v>
       </c>
       <c r="E200">
-        <v>10.38653705362939</v>
+        <v>12.03394341032428</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>14.9999999092348</v>
+        <v>14.945107269859291</v>
       </c>
       <c r="B201">
-        <v>0.83325793055932718</v>
+        <v>0.88474583147116448</v>
       </c>
       <c r="C201">
-        <v>42.150058528305223</v>
+        <v>52.864480536938792</v>
       </c>
       <c r="D201">
-        <v>0.85573402666469578</v>
+        <v>0.72900099707553567</v>
       </c>
       <c r="E201">
-        <v>10.694612010915479</v>
+        <v>12.41567360616558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>